<commit_message>
Updated tests to reflect updated plate parsing methodology (new min-max scaling etc.).
</commit_message>
<xml_diff>
--- a/tests/Test_plates/Test_1/Test_plate_1_repeat_1.xlsx
+++ b/tests/Test_plates/Test_1/Test_plate_1_repeat_1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ks17361/Lab_work_Dek_Woolfson/BADASS/sensing_array_paper_2019/tests/Test_plates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ks17361/Lab_work_Dek_Woolfson/BADASS/array_sensing/tests/Test_plates/Test_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B51CA6-224D-2F48-803E-5A42A6F19E5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33FE0B94-E736-0644-AF6E-32395C5C71B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="2440" windowWidth="27300" windowHeight="14240" xr2:uid="{3108E363-480C-1C4C-B971-293712F19C9B}"/>
   </bookViews>
@@ -24,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="61">
   <si>
     <t>Peptide layout</t>
   </si>
@@ -209,9 +211,6 @@
   </si>
   <si>
     <t>O:P</t>
-  </si>
-  <si>
-    <t>Median min fluor readings</t>
   </si>
   <si>
     <t>Median max fluor (blank) readings</t>
@@ -224,7 +223,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -244,13 +243,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -335,7 +327,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -346,9 +338,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -410,13 +399,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -738,8 +723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1E78E01-51D6-624A-8582-548840E6FF26}">
   <dimension ref="A3:Y77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I66" sqref="I66"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -867,76 +852,76 @@
       <c r="A16" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16" s="8">
         <v>155</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="9">
         <v>9290</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="9">
         <v>166</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="9">
         <v>375</v>
       </c>
-      <c r="F16" s="10">
+      <c r="F16" s="9">
         <v>9358</v>
       </c>
-      <c r="G16" s="10">
+      <c r="G16" s="9">
         <v>10367</v>
       </c>
-      <c r="H16" s="10">
+      <c r="H16" s="9">
         <v>8292</v>
       </c>
-      <c r="I16" s="10">
+      <c r="I16" s="9">
         <v>1668</v>
       </c>
       <c r="J16" s="5">
         <v>117</v>
       </c>
-      <c r="K16" s="7">
+      <c r="K16" s="6">
         <v>11106</v>
       </c>
-      <c r="L16" s="7">
+      <c r="L16" s="6">
         <v>149</v>
       </c>
-      <c r="M16" s="7">
+      <c r="M16" s="6">
         <v>298</v>
       </c>
-      <c r="N16" s="7">
+      <c r="N16" s="6">
         <v>8773</v>
       </c>
-      <c r="O16" s="7">
+      <c r="O16" s="6">
         <v>9308</v>
       </c>
-      <c r="P16" s="7">
+      <c r="P16" s="6">
         <v>8550</v>
       </c>
-      <c r="Q16" s="7">
+      <c r="Q16" s="6">
         <v>2193</v>
       </c>
-      <c r="R16" s="21">
+      <c r="R16" s="20">
         <v>164</v>
       </c>
-      <c r="S16" s="22">
+      <c r="S16" s="21">
         <v>10021</v>
       </c>
-      <c r="T16" s="22">
+      <c r="T16" s="21">
         <v>169</v>
       </c>
-      <c r="U16" s="22">
+      <c r="U16" s="21">
         <v>515</v>
       </c>
-      <c r="V16" s="22">
+      <c r="V16" s="21">
         <v>14171</v>
       </c>
-      <c r="W16" s="22">
+      <c r="W16" s="21">
         <v>13326</v>
       </c>
-      <c r="X16" s="22">
+      <c r="X16" s="21">
         <v>13394</v>
       </c>
-      <c r="Y16" s="22">
+      <c r="Y16" s="21">
         <v>3302</v>
       </c>
     </row>
@@ -944,76 +929,76 @@
       <c r="A17" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="11">
+      <c r="B17" s="10">
         <v>2178</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C17" s="11">
         <v>590</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17" s="11">
         <v>763</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="11">
         <v>4370</v>
       </c>
-      <c r="F17" s="12">
+      <c r="F17" s="11">
         <v>1420</v>
       </c>
-      <c r="G17" s="12">
+      <c r="G17" s="11">
         <v>1481</v>
       </c>
-      <c r="H17" s="12">
+      <c r="H17" s="11">
         <v>3988</v>
       </c>
-      <c r="I17" s="12">
+      <c r="I17" s="11">
         <v>228</v>
       </c>
       <c r="J17" s="5">
         <v>4612</v>
       </c>
-      <c r="K17" s="7">
+      <c r="K17" s="6">
         <v>1063</v>
       </c>
-      <c r="L17" s="7">
+      <c r="L17" s="6">
         <v>1025</v>
       </c>
-      <c r="M17" s="7">
+      <c r="M17" s="6">
         <v>3231</v>
       </c>
-      <c r="N17" s="7">
+      <c r="N17" s="6">
         <v>4999</v>
       </c>
-      <c r="O17" s="7">
+      <c r="O17" s="6">
         <v>7472</v>
       </c>
-      <c r="P17" s="7">
+      <c r="P17" s="6">
         <v>8723</v>
       </c>
-      <c r="Q17" s="7">
+      <c r="Q17" s="6">
         <v>235</v>
       </c>
-      <c r="R17" s="19">
+      <c r="R17" s="18">
         <v>4499</v>
       </c>
-      <c r="S17" s="20">
+      <c r="S17" s="19">
         <v>868</v>
       </c>
-      <c r="T17" s="20">
+      <c r="T17" s="19">
         <v>797</v>
       </c>
-      <c r="U17" s="20">
+      <c r="U17" s="19">
         <v>5134</v>
       </c>
-      <c r="V17" s="20">
+      <c r="V17" s="19">
         <v>3714</v>
       </c>
-      <c r="W17" s="20">
+      <c r="W17" s="19">
         <v>7207</v>
       </c>
-      <c r="X17" s="20">
+      <c r="X17" s="19">
         <v>9255</v>
       </c>
-      <c r="Y17" s="20">
+      <c r="Y17" s="19">
         <v>392</v>
       </c>
     </row>
@@ -1021,76 +1006,76 @@
       <c r="A18" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="14">
+      <c r="B18" s="13">
         <v>163</v>
       </c>
-      <c r="C18" s="15">
+      <c r="C18" s="14">
         <v>5406</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="14">
         <v>176</v>
       </c>
-      <c r="E18" s="15">
+      <c r="E18" s="14">
         <v>344</v>
       </c>
-      <c r="F18" s="15">
+      <c r="F18" s="14">
         <v>6666</v>
       </c>
-      <c r="G18" s="15">
+      <c r="G18" s="14">
         <v>13293</v>
       </c>
-      <c r="H18" s="15">
+      <c r="H18" s="14">
         <v>10514</v>
       </c>
-      <c r="I18" s="15">
+      <c r="I18" s="14">
         <v>2114</v>
       </c>
-      <c r="J18" s="19">
+      <c r="J18" s="18">
         <v>166</v>
       </c>
-      <c r="K18" s="20">
+      <c r="K18" s="19">
         <v>12908</v>
       </c>
-      <c r="L18" s="20">
+      <c r="L18" s="19">
         <v>174</v>
       </c>
-      <c r="M18" s="20">
+      <c r="M18" s="19">
         <v>592</v>
       </c>
-      <c r="N18" s="20">
+      <c r="N18" s="19">
         <v>17411</v>
       </c>
-      <c r="O18" s="20">
+      <c r="O18" s="19">
         <v>16849</v>
       </c>
-      <c r="P18" s="20">
+      <c r="P18" s="19">
         <v>13507</v>
       </c>
-      <c r="Q18" s="20">
+      <c r="Q18" s="19">
         <v>3171</v>
       </c>
-      <c r="R18" s="26">
+      <c r="R18" s="25">
         <v>159</v>
       </c>
-      <c r="S18" s="27">
+      <c r="S18" s="26">
         <v>5395</v>
       </c>
-      <c r="T18" s="27">
+      <c r="T18" s="26">
         <v>165</v>
       </c>
-      <c r="U18" s="27">
+      <c r="U18" s="26">
         <v>245</v>
       </c>
-      <c r="V18" s="27">
+      <c r="V18" s="26">
         <v>5012</v>
       </c>
-      <c r="W18" s="27">
+      <c r="W18" s="26">
         <v>5417</v>
       </c>
-      <c r="X18" s="27">
+      <c r="X18" s="26">
         <v>6066</v>
       </c>
-      <c r="Y18" s="27">
+      <c r="Y18" s="26">
         <v>1307</v>
       </c>
     </row>
@@ -1098,76 +1083,76 @@
       <c r="A19" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="16">
+      <c r="B19" s="15">
         <v>2736</v>
       </c>
-      <c r="C19" s="17">
+      <c r="C19" s="16">
         <v>625</v>
       </c>
-      <c r="D19" s="17">
+      <c r="D19" s="16">
         <v>627</v>
       </c>
-      <c r="E19" s="17">
+      <c r="E19" s="16">
         <v>4659</v>
       </c>
-      <c r="F19" s="17">
+      <c r="F19" s="16">
         <v>1403</v>
       </c>
-      <c r="G19" s="17">
+      <c r="G19" s="16">
         <v>1418</v>
       </c>
-      <c r="H19" s="17">
+      <c r="H19" s="16">
         <v>4651</v>
       </c>
-      <c r="I19" s="17">
+      <c r="I19" s="16">
         <v>292</v>
       </c>
-      <c r="J19" s="19">
+      <c r="J19" s="18">
         <v>5138</v>
       </c>
-      <c r="K19" s="20">
+      <c r="K19" s="19">
         <v>1142</v>
       </c>
-      <c r="L19" s="20">
+      <c r="L19" s="19">
         <v>956</v>
       </c>
-      <c r="M19" s="20">
+      <c r="M19" s="19">
         <v>6219</v>
       </c>
-      <c r="N19" s="20">
+      <c r="N19" s="19">
         <v>5013</v>
       </c>
-      <c r="O19" s="20">
+      <c r="O19" s="19">
         <v>9836</v>
       </c>
-      <c r="P19" s="20">
+      <c r="P19" s="19">
         <v>9242</v>
       </c>
-      <c r="Q19" s="20">
+      <c r="Q19" s="19">
         <v>416</v>
       </c>
-      <c r="R19" s="24">
+      <c r="R19" s="23">
         <v>2048</v>
       </c>
-      <c r="S19" s="25">
+      <c r="S19" s="24">
         <v>437</v>
       </c>
-      <c r="T19" s="25">
+      <c r="T19" s="24">
         <v>357</v>
       </c>
-      <c r="U19" s="25">
+      <c r="U19" s="24">
         <v>1238</v>
       </c>
-      <c r="V19" s="25">
+      <c r="V19" s="24">
         <v>849</v>
       </c>
-      <c r="W19" s="25">
+      <c r="W19" s="24">
         <v>1783</v>
       </c>
-      <c r="X19" s="25">
+      <c r="X19" s="24">
         <v>2443</v>
       </c>
-      <c r="Y19" s="25">
+      <c r="Y19" s="24">
         <v>171</v>
       </c>
     </row>
@@ -1175,76 +1160,76 @@
       <c r="A20" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="16">
+      <c r="B20" s="15">
         <v>170</v>
       </c>
-      <c r="C20" s="17">
+      <c r="C20" s="16">
         <v>7097</v>
       </c>
-      <c r="D20" s="17">
+      <c r="D20" s="16">
         <v>170</v>
       </c>
-      <c r="E20" s="17">
+      <c r="E20" s="16">
         <v>372</v>
       </c>
-      <c r="F20" s="17">
+      <c r="F20" s="16">
         <v>8117</v>
       </c>
-      <c r="G20" s="17">
+      <c r="G20" s="16">
         <v>16028</v>
       </c>
-      <c r="H20" s="17">
+      <c r="H20" s="16">
         <v>10209</v>
       </c>
-      <c r="I20" s="17">
+      <c r="I20" s="16">
         <v>2157</v>
       </c>
-      <c r="J20" s="24">
+      <c r="J20" s="23">
         <v>164</v>
       </c>
-      <c r="K20" s="25">
+      <c r="K20" s="24">
         <v>7468</v>
       </c>
-      <c r="L20" s="25">
+      <c r="L20" s="24">
         <v>167</v>
       </c>
-      <c r="M20" s="25">
+      <c r="M20" s="24">
         <v>283</v>
       </c>
-      <c r="N20" s="25">
+      <c r="N20" s="24">
         <v>6317</v>
       </c>
-      <c r="O20" s="25">
+      <c r="O20" s="24">
         <v>7315</v>
       </c>
-      <c r="P20" s="25">
+      <c r="P20" s="24">
         <v>6273</v>
       </c>
-      <c r="Q20" s="25">
+      <c r="Q20" s="24">
         <v>1324</v>
       </c>
-      <c r="R20" s="24">
+      <c r="R20" s="23">
         <v>160</v>
       </c>
-      <c r="S20" s="25">
+      <c r="S20" s="24">
         <v>7702</v>
       </c>
-      <c r="T20" s="25">
+      <c r="T20" s="24">
         <v>165</v>
       </c>
-      <c r="U20" s="25">
+      <c r="U20" s="24">
         <v>282</v>
       </c>
-      <c r="V20" s="25">
+      <c r="V20" s="24">
         <v>6593</v>
       </c>
-      <c r="W20" s="25">
+      <c r="W20" s="24">
         <v>7236</v>
       </c>
-      <c r="X20" s="25">
+      <c r="X20" s="24">
         <v>6169</v>
       </c>
-      <c r="Y20" s="25">
+      <c r="Y20" s="24">
         <v>1421</v>
       </c>
     </row>
@@ -1252,76 +1237,76 @@
       <c r="A21" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="16">
+      <c r="B21" s="15">
         <v>3187</v>
       </c>
-      <c r="C21" s="17">
+      <c r="C21" s="16">
         <v>780</v>
       </c>
-      <c r="D21" s="17">
+      <c r="D21" s="16">
         <v>621</v>
       </c>
-      <c r="E21" s="17">
+      <c r="E21" s="16">
         <v>4698</v>
       </c>
-      <c r="F21" s="17">
+      <c r="F21" s="16">
         <v>1942</v>
       </c>
-      <c r="G21" s="17">
+      <c r="G21" s="16">
         <v>2357</v>
       </c>
-      <c r="H21" s="17">
+      <c r="H21" s="16">
         <v>4709</v>
       </c>
-      <c r="I21" s="17">
+      <c r="I21" s="16">
         <v>282</v>
       </c>
-      <c r="J21" s="24">
+      <c r="J21" s="23">
         <v>2549</v>
       </c>
-      <c r="K21" s="25">
+      <c r="K21" s="24">
         <v>587</v>
       </c>
-      <c r="L21" s="25">
+      <c r="L21" s="24">
         <v>433</v>
       </c>
-      <c r="M21" s="25">
+      <c r="M21" s="24">
         <v>1676</v>
       </c>
-      <c r="N21" s="25">
+      <c r="N21" s="24">
         <v>1479</v>
       </c>
-      <c r="O21" s="25">
+      <c r="O21" s="24">
         <v>3359</v>
       </c>
-      <c r="P21" s="25">
+      <c r="P21" s="24">
         <v>2430</v>
       </c>
-      <c r="Q21" s="25">
+      <c r="Q21" s="24">
         <v>180</v>
       </c>
-      <c r="R21" s="24">
+      <c r="R21" s="23">
         <v>2464</v>
       </c>
-      <c r="S21" s="25">
+      <c r="S21" s="24">
         <v>653</v>
       </c>
-      <c r="T21" s="25">
+      <c r="T21" s="24">
         <v>408</v>
       </c>
-      <c r="U21" s="25">
+      <c r="U21" s="24">
         <v>1445</v>
       </c>
-      <c r="V21" s="25">
+      <c r="V21" s="24">
         <v>1577</v>
       </c>
-      <c r="W21" s="25">
+      <c r="W21" s="24">
         <v>3326</v>
       </c>
-      <c r="X21" s="25">
+      <c r="X21" s="24">
         <v>2416</v>
       </c>
-      <c r="Y21" s="25">
+      <c r="Y21" s="24">
         <v>172</v>
       </c>
     </row>
@@ -1329,76 +1314,76 @@
       <c r="A22" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="16">
+      <c r="B22" s="15">
         <v>164</v>
       </c>
-      <c r="C22" s="17">
+      <c r="C22" s="16">
         <v>7287</v>
       </c>
-      <c r="D22" s="17">
+      <c r="D22" s="16">
         <v>168</v>
       </c>
-      <c r="E22" s="17">
+      <c r="E22" s="16">
         <v>370</v>
       </c>
-      <c r="F22" s="17">
+      <c r="F22" s="16">
         <v>7889</v>
       </c>
-      <c r="G22" s="17">
+      <c r="G22" s="16">
         <v>16022</v>
       </c>
-      <c r="H22" s="17">
+      <c r="H22" s="16">
         <v>9775</v>
       </c>
-      <c r="I22" s="17">
+      <c r="I22" s="16">
         <v>2183</v>
       </c>
-      <c r="J22" s="19">
+      <c r="J22" s="18">
         <v>161</v>
       </c>
-      <c r="K22" s="20">
+      <c r="K22" s="19">
         <v>13346</v>
       </c>
-      <c r="L22" s="20">
+      <c r="L22" s="19">
         <v>171</v>
       </c>
-      <c r="M22" s="20">
+      <c r="M22" s="19">
         <v>600</v>
       </c>
-      <c r="N22" s="20">
+      <c r="N22" s="19">
         <v>17275</v>
       </c>
-      <c r="O22" s="20">
+      <c r="O22" s="19">
         <v>16770</v>
       </c>
-      <c r="P22" s="20">
+      <c r="P22" s="19">
         <v>13642</v>
       </c>
-      <c r="Q22" s="20">
+      <c r="Q22" s="19">
         <v>3150</v>
       </c>
       <c r="R22" s="5">
         <v>120</v>
       </c>
-      <c r="S22" s="7">
+      <c r="S22" s="6">
         <v>17841</v>
       </c>
-      <c r="T22" s="7">
+      <c r="T22" s="6">
         <v>131</v>
       </c>
-      <c r="U22" s="7">
+      <c r="U22" s="6">
         <v>600</v>
       </c>
-      <c r="V22" s="7">
+      <c r="V22" s="6">
         <v>18407</v>
       </c>
-      <c r="W22" s="7">
+      <c r="W22" s="6">
         <v>17572</v>
       </c>
-      <c r="X22" s="7">
+      <c r="X22" s="6">
         <v>15398</v>
       </c>
-      <c r="Y22" s="7">
+      <c r="Y22" s="6">
         <v>4280</v>
       </c>
     </row>
@@ -1406,76 +1391,76 @@
       <c r="A23" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="16">
+      <c r="B23" s="15">
         <v>3383</v>
       </c>
-      <c r="C23" s="17">
+      <c r="C23" s="16">
         <v>873</v>
       </c>
-      <c r="D23" s="17">
+      <c r="D23" s="16">
         <v>586</v>
       </c>
-      <c r="E23" s="17">
+      <c r="E23" s="16">
         <v>3498</v>
       </c>
-      <c r="F23" s="17">
+      <c r="F23" s="16">
         <v>1969</v>
       </c>
-      <c r="G23" s="17">
+      <c r="G23" s="16">
         <v>2145</v>
       </c>
-      <c r="H23" s="17">
+      <c r="H23" s="16">
         <v>4554</v>
       </c>
-      <c r="I23" s="17">
+      <c r="I23" s="16">
         <v>293</v>
       </c>
-      <c r="J23" s="19">
+      <c r="J23" s="18">
         <v>5491</v>
       </c>
-      <c r="K23" s="20">
+      <c r="K23" s="19">
         <v>1198</v>
       </c>
-      <c r="L23" s="20">
+      <c r="L23" s="19">
         <v>943</v>
       </c>
-      <c r="M23" s="20">
+      <c r="M23" s="19">
         <v>6296</v>
       </c>
-      <c r="N23" s="20">
+      <c r="N23" s="19">
         <v>4786</v>
       </c>
-      <c r="O23" s="20">
+      <c r="O23" s="19">
         <v>9728</v>
       </c>
-      <c r="P23" s="20">
+      <c r="P23" s="19">
         <v>8754</v>
       </c>
-      <c r="Q23" s="20">
+      <c r="Q23" s="19">
         <v>409</v>
       </c>
       <c r="R23" s="5">
         <v>6112</v>
       </c>
-      <c r="S23" s="7">
+      <c r="S23" s="6">
         <v>1485</v>
       </c>
-      <c r="T23" s="7">
+      <c r="T23" s="6">
         <v>1619</v>
       </c>
-      <c r="U23" s="7">
+      <c r="U23" s="6">
         <v>9133</v>
       </c>
-      <c r="V23" s="7">
+      <c r="V23" s="6">
         <v>7668</v>
       </c>
-      <c r="W23" s="7">
+      <c r="W23" s="6">
         <v>13545</v>
       </c>
-      <c r="X23" s="7">
+      <c r="X23" s="6">
         <v>14580</v>
       </c>
-      <c r="Y23" s="7">
+      <c r="Y23" s="6">
         <v>571</v>
       </c>
     </row>
@@ -1483,76 +1468,76 @@
       <c r="A24" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="19">
+      <c r="B24" s="18">
         <v>167</v>
       </c>
-      <c r="C24" s="20">
+      <c r="C24" s="19">
         <v>12652</v>
       </c>
-      <c r="D24" s="20">
+      <c r="D24" s="19">
         <v>178</v>
       </c>
-      <c r="E24" s="20">
+      <c r="E24" s="19">
         <v>598</v>
       </c>
-      <c r="F24" s="20">
+      <c r="F24" s="19">
         <v>17270</v>
       </c>
-      <c r="G24" s="20">
+      <c r="G24" s="19">
         <v>16455</v>
       </c>
-      <c r="H24" s="20">
+      <c r="H24" s="19">
         <v>13531</v>
       </c>
-      <c r="I24" s="20">
+      <c r="I24" s="19">
         <v>3266</v>
       </c>
       <c r="J24" s="5">
         <v>135</v>
       </c>
-      <c r="K24" s="7">
+      <c r="K24" s="6">
         <v>11947</v>
       </c>
-      <c r="L24" s="7">
+      <c r="L24" s="6">
         <v>146</v>
       </c>
-      <c r="M24" s="7">
+      <c r="M24" s="6">
         <v>419</v>
       </c>
-      <c r="N24" s="7">
+      <c r="N24" s="6">
         <v>11195</v>
       </c>
-      <c r="O24" s="7">
+      <c r="O24" s="6">
         <v>19921</v>
       </c>
-      <c r="P24" s="7">
+      <c r="P24" s="6">
         <v>13121</v>
       </c>
-      <c r="Q24" s="7">
+      <c r="Q24" s="6">
         <v>2618</v>
       </c>
-      <c r="R24" s="11">
+      <c r="R24" s="10">
         <v>151</v>
       </c>
-      <c r="S24" s="12">
+      <c r="S24" s="11">
         <v>11616</v>
       </c>
-      <c r="T24" s="12">
+      <c r="T24" s="11">
         <v>154</v>
       </c>
-      <c r="U24" s="12">
+      <c r="U24" s="11">
         <v>391</v>
       </c>
-      <c r="V24" s="12">
+      <c r="V24" s="11">
         <v>11195</v>
       </c>
-      <c r="W24" s="12">
+      <c r="W24" s="11">
         <v>12494</v>
       </c>
-      <c r="X24" s="12">
+      <c r="X24" s="11">
         <v>8548</v>
       </c>
-      <c r="Y24" s="12">
+      <c r="Y24" s="11">
         <v>1566</v>
       </c>
     </row>
@@ -1560,76 +1545,76 @@
       <c r="A25" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="19">
+      <c r="B25" s="18">
         <v>5367</v>
       </c>
-      <c r="C25" s="20">
+      <c r="C25" s="19">
         <v>1213</v>
       </c>
-      <c r="D25" s="20">
+      <c r="D25" s="19">
         <v>1080</v>
       </c>
-      <c r="E25" s="20">
+      <c r="E25" s="19">
         <v>6331</v>
       </c>
-      <c r="F25" s="20">
+      <c r="F25" s="19">
         <v>4980</v>
       </c>
-      <c r="G25" s="20">
+      <c r="G25" s="19">
         <v>9966</v>
       </c>
-      <c r="H25" s="20">
+      <c r="H25" s="19">
         <v>9440</v>
       </c>
-      <c r="I25" s="20">
+      <c r="I25" s="19">
         <v>462</v>
       </c>
       <c r="J25" s="5">
         <v>5405</v>
       </c>
-      <c r="K25" s="7">
+      <c r="K25" s="6">
         <v>1321</v>
       </c>
-      <c r="L25" s="7">
+      <c r="L25" s="6">
         <v>1736</v>
       </c>
-      <c r="M25" s="7">
+      <c r="M25" s="6">
         <v>8902</v>
       </c>
-      <c r="N25" s="7">
+      <c r="N25" s="6">
         <v>5720</v>
       </c>
-      <c r="O25" s="7">
+      <c r="O25" s="6">
         <v>7068</v>
       </c>
-      <c r="P25" s="7">
+      <c r="P25" s="6">
         <v>12413</v>
       </c>
-      <c r="Q25" s="7">
+      <c r="Q25" s="6">
         <v>475</v>
       </c>
-      <c r="R25" s="11">
+      <c r="R25" s="10">
         <v>2532</v>
       </c>
-      <c r="S25" s="12">
+      <c r="S25" s="11">
         <v>740</v>
       </c>
-      <c r="T25" s="12">
+      <c r="T25" s="11">
         <v>809</v>
       </c>
-      <c r="U25" s="12">
+      <c r="U25" s="11">
         <v>4510</v>
       </c>
-      <c r="V25" s="12">
+      <c r="V25" s="11">
         <v>2135</v>
       </c>
-      <c r="W25" s="12">
+      <c r="W25" s="11">
         <v>2372</v>
       </c>
-      <c r="X25" s="12">
+      <c r="X25" s="11">
         <v>4256</v>
       </c>
-      <c r="Y25" s="12">
+      <c r="Y25" s="11">
         <v>232</v>
       </c>
     </row>
@@ -1637,76 +1622,76 @@
       <c r="A26" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="16">
+      <c r="B26" s="15">
         <v>161</v>
       </c>
-      <c r="C26" s="17">
+      <c r="C26" s="16">
         <v>8129</v>
       </c>
-      <c r="D26" s="17">
+      <c r="D26" s="16">
         <v>176</v>
       </c>
-      <c r="E26" s="17">
+      <c r="E26" s="16">
         <v>381</v>
       </c>
-      <c r="F26" s="17">
+      <c r="F26" s="16">
         <v>8586</v>
       </c>
-      <c r="G26" s="17">
+      <c r="G26" s="16">
         <v>16468</v>
       </c>
-      <c r="H26" s="17">
+      <c r="H26" s="16">
         <v>10576</v>
       </c>
-      <c r="I26" s="17">
+      <c r="I26" s="16">
         <v>2203</v>
       </c>
-      <c r="J26" s="19">
+      <c r="J26" s="18">
         <v>166</v>
       </c>
-      <c r="K26" s="20">
+      <c r="K26" s="19">
         <v>13119</v>
       </c>
-      <c r="L26" s="20">
+      <c r="L26" s="19">
         <v>174</v>
       </c>
-      <c r="M26" s="20">
+      <c r="M26" s="19">
         <v>597</v>
       </c>
-      <c r="N26" s="20">
+      <c r="N26" s="19">
         <v>17943</v>
       </c>
-      <c r="O26" s="20">
+      <c r="O26" s="19">
         <v>16244</v>
       </c>
-      <c r="P26" s="20">
+      <c r="P26" s="19">
         <v>13570</v>
       </c>
-      <c r="Q26" s="20">
+      <c r="Q26" s="19">
         <v>3247</v>
       </c>
       <c r="R26" s="5">
         <v>110</v>
       </c>
-      <c r="S26" s="7">
+      <c r="S26" s="6">
         <v>14665</v>
       </c>
-      <c r="T26" s="7">
+      <c r="T26" s="6">
         <v>135</v>
       </c>
-      <c r="U26" s="7">
+      <c r="U26" s="6">
         <v>429</v>
       </c>
-      <c r="V26" s="7">
+      <c r="V26" s="6">
         <v>13902</v>
       </c>
-      <c r="W26" s="7">
+      <c r="W26" s="6">
         <v>15203</v>
       </c>
-      <c r="X26" s="7">
+      <c r="X26" s="6">
         <v>10145</v>
       </c>
-      <c r="Y26" s="7">
+      <c r="Y26" s="6">
         <v>2020</v>
       </c>
     </row>
@@ -1714,76 +1699,76 @@
       <c r="A27" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="16">
+      <c r="B27" s="15">
         <v>3480</v>
       </c>
-      <c r="C27" s="17">
+      <c r="C27" s="16">
         <v>880</v>
       </c>
-      <c r="D27" s="17">
+      <c r="D27" s="16">
         <v>666</v>
       </c>
-      <c r="E27" s="17">
+      <c r="E27" s="16">
         <v>5360</v>
       </c>
-      <c r="F27" s="17">
+      <c r="F27" s="16">
         <v>2034</v>
       </c>
-      <c r="G27" s="17">
+      <c r="G27" s="16">
         <v>2206</v>
       </c>
-      <c r="H27" s="17">
+      <c r="H27" s="16">
         <v>5169</v>
       </c>
-      <c r="I27" s="17">
+      <c r="I27" s="16">
         <v>291</v>
       </c>
-      <c r="J27" s="19">
+      <c r="J27" s="18">
         <v>5685</v>
       </c>
-      <c r="K27" s="20">
+      <c r="K27" s="19">
         <v>1114</v>
       </c>
-      <c r="L27" s="20">
+      <c r="L27" s="19">
         <v>982</v>
       </c>
-      <c r="M27" s="20">
+      <c r="M27" s="19">
         <v>6465</v>
       </c>
-      <c r="N27" s="20">
+      <c r="N27" s="19">
         <v>5001</v>
       </c>
-      <c r="O27" s="20">
+      <c r="O27" s="19">
         <v>10054</v>
       </c>
-      <c r="P27" s="20">
+      <c r="P27" s="19">
         <v>9450</v>
       </c>
-      <c r="Q27" s="20">
+      <c r="Q27" s="19">
         <v>457</v>
       </c>
       <c r="R27" s="5">
         <v>3565</v>
       </c>
-      <c r="S27" s="7">
+      <c r="S27" s="6">
         <v>1118</v>
       </c>
-      <c r="T27" s="7">
+      <c r="T27" s="6">
         <v>1857</v>
       </c>
-      <c r="U27" s="7">
+      <c r="U27" s="6">
         <v>6636</v>
       </c>
-      <c r="V27" s="7">
+      <c r="V27" s="6">
         <v>4768</v>
       </c>
-      <c r="W27" s="7">
+      <c r="W27" s="6">
         <v>6081</v>
       </c>
-      <c r="X27" s="7">
+      <c r="X27" s="6">
         <v>9523</v>
       </c>
-      <c r="Y27" s="7">
+      <c r="Y27" s="6">
         <v>311</v>
       </c>
     </row>
@@ -1791,76 +1776,76 @@
       <c r="A28" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="24">
+      <c r="B28" s="23">
         <v>166</v>
       </c>
-      <c r="C28" s="25">
+      <c r="C28" s="24">
         <v>7388</v>
       </c>
-      <c r="D28" s="25">
+      <c r="D28" s="24">
         <v>174</v>
       </c>
-      <c r="E28" s="25">
+      <c r="E28" s="24">
         <v>295</v>
       </c>
-      <c r="F28" s="25">
+      <c r="F28" s="24">
         <v>6250</v>
       </c>
-      <c r="G28" s="25">
+      <c r="G28" s="24">
         <v>7372</v>
       </c>
-      <c r="H28" s="25">
+      <c r="H28" s="24">
         <v>6244</v>
       </c>
-      <c r="I28" s="25">
+      <c r="I28" s="24">
         <v>1429</v>
       </c>
-      <c r="J28" s="11">
+      <c r="J28" s="10">
         <v>150</v>
       </c>
-      <c r="K28" s="12">
+      <c r="K28" s="11">
         <v>11546</v>
       </c>
-      <c r="L28" s="12">
+      <c r="L28" s="11">
         <v>157</v>
       </c>
-      <c r="M28" s="12">
+      <c r="M28" s="11">
         <v>400</v>
       </c>
-      <c r="N28" s="12">
+      <c r="N28" s="11">
         <v>11288</v>
       </c>
-      <c r="O28" s="12">
+      <c r="O28" s="11">
         <v>12614</v>
       </c>
-      <c r="P28" s="12">
+      <c r="P28" s="11">
         <v>8808</v>
       </c>
-      <c r="Q28" s="12">
+      <c r="Q28" s="11">
         <v>1732</v>
       </c>
-      <c r="R28" s="24">
+      <c r="R28" s="23">
         <v>172</v>
       </c>
-      <c r="S28" s="25">
+      <c r="S28" s="24">
         <v>7447</v>
       </c>
-      <c r="T28" s="25">
+      <c r="T28" s="24">
         <v>174</v>
       </c>
-      <c r="U28" s="25">
+      <c r="U28" s="24">
         <v>282</v>
       </c>
-      <c r="V28" s="25">
+      <c r="V28" s="24">
         <v>6376</v>
       </c>
-      <c r="W28" s="25">
+      <c r="W28" s="24">
         <v>7011</v>
       </c>
-      <c r="X28" s="25">
+      <c r="X28" s="24">
         <v>6220</v>
       </c>
-      <c r="Y28" s="25">
+      <c r="Y28" s="24">
         <v>1368</v>
       </c>
     </row>
@@ -1868,76 +1853,76 @@
       <c r="A29" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B29" s="24">
+      <c r="B29" s="23">
         <v>2548</v>
       </c>
-      <c r="C29" s="25">
+      <c r="C29" s="24">
         <v>692</v>
       </c>
-      <c r="D29" s="25">
+      <c r="D29" s="24">
         <v>429</v>
       </c>
-      <c r="E29" s="25">
+      <c r="E29" s="24">
         <v>1649</v>
       </c>
-      <c r="F29" s="25">
+      <c r="F29" s="24">
         <v>1567</v>
       </c>
-      <c r="G29" s="25">
+      <c r="G29" s="24">
         <v>3096</v>
       </c>
-      <c r="H29" s="25">
+      <c r="H29" s="24">
         <v>2401</v>
       </c>
-      <c r="I29" s="25">
+      <c r="I29" s="24">
         <v>182</v>
       </c>
-      <c r="J29" s="11">
+      <c r="J29" s="10">
         <v>2629</v>
       </c>
-      <c r="K29" s="12">
+      <c r="K29" s="11">
         <v>765</v>
       </c>
-      <c r="L29" s="12">
+      <c r="L29" s="11">
         <v>819</v>
       </c>
-      <c r="M29" s="12">
+      <c r="M29" s="11">
         <v>4635</v>
       </c>
-      <c r="N29" s="12">
+      <c r="N29" s="11">
         <v>2174</v>
       </c>
-      <c r="O29" s="12">
+      <c r="O29" s="11">
         <v>2346</v>
       </c>
-      <c r="P29" s="12">
+      <c r="P29" s="11">
         <v>4491</v>
       </c>
-      <c r="Q29" s="12">
+      <c r="Q29" s="11">
         <v>239</v>
       </c>
-      <c r="R29" s="24">
+      <c r="R29" s="23">
         <v>2311</v>
       </c>
-      <c r="S29" s="25">
+      <c r="S29" s="24">
         <v>574</v>
       </c>
-      <c r="T29" s="25">
+      <c r="T29" s="24">
         <v>436</v>
       </c>
-      <c r="U29" s="25">
+      <c r="U29" s="24">
         <v>1559</v>
       </c>
-      <c r="V29" s="25">
+      <c r="V29" s="24">
         <v>1475</v>
       </c>
-      <c r="W29" s="25">
+      <c r="W29" s="24">
         <v>3083</v>
       </c>
-      <c r="X29" s="25">
+      <c r="X29" s="24">
         <v>2418</v>
       </c>
-      <c r="Y29" s="25">
+      <c r="Y29" s="24">
         <v>182</v>
       </c>
     </row>
@@ -1945,76 +1930,76 @@
       <c r="A30" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B30" s="11">
+      <c r="B30" s="10">
         <v>155</v>
       </c>
-      <c r="C30" s="12">
+      <c r="C30" s="11">
         <v>11343</v>
       </c>
-      <c r="D30" s="12">
+      <c r="D30" s="11">
         <v>164</v>
       </c>
-      <c r="E30" s="12">
+      <c r="E30" s="11">
         <v>394</v>
       </c>
-      <c r="F30" s="12">
+      <c r="F30" s="11">
         <v>11055</v>
       </c>
-      <c r="G30" s="12">
+      <c r="G30" s="11">
         <v>12251</v>
       </c>
-      <c r="H30" s="12">
+      <c r="H30" s="11">
         <v>8777</v>
       </c>
-      <c r="I30" s="12">
+      <c r="I30" s="11">
         <v>1730</v>
       </c>
-      <c r="J30" s="16">
+      <c r="J30" s="15">
         <v>169</v>
       </c>
-      <c r="K30" s="17">
+      <c r="K30" s="16">
         <v>7406</v>
       </c>
-      <c r="L30" s="17">
+      <c r="L30" s="16">
         <v>173</v>
       </c>
-      <c r="M30" s="17">
+      <c r="M30" s="16">
         <v>359</v>
       </c>
-      <c r="N30" s="17">
+      <c r="N30" s="16">
         <v>8631</v>
       </c>
-      <c r="O30" s="17">
+      <c r="O30" s="16">
         <v>16813</v>
       </c>
-      <c r="P30" s="17">
+      <c r="P30" s="16">
         <v>10667</v>
       </c>
-      <c r="Q30" s="17">
+      <c r="Q30" s="16">
         <v>2151</v>
       </c>
-      <c r="R30" s="11">
+      <c r="R30" s="10">
         <v>150</v>
       </c>
-      <c r="S30" s="12">
+      <c r="S30" s="11">
         <v>11784</v>
       </c>
-      <c r="T30" s="12">
+      <c r="T30" s="11">
         <v>163</v>
       </c>
-      <c r="U30" s="12">
+      <c r="U30" s="11">
         <v>409</v>
       </c>
-      <c r="V30" s="12">
+      <c r="V30" s="11">
         <v>11042</v>
       </c>
-      <c r="W30" s="12">
+      <c r="W30" s="11">
         <v>12808</v>
       </c>
-      <c r="X30" s="12">
+      <c r="X30" s="11">
         <v>9220</v>
       </c>
-      <c r="Y30" s="12">
+      <c r="Y30" s="11">
         <v>1714</v>
       </c>
     </row>
@@ -2022,337 +2007,108 @@
       <c r="A31" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B31" s="11">
+      <c r="B31" s="10">
         <v>2731</v>
       </c>
-      <c r="C31" s="12">
+      <c r="C31" s="11">
         <v>715</v>
       </c>
-      <c r="D31" s="12">
+      <c r="D31" s="11">
         <v>807</v>
       </c>
-      <c r="E31" s="12">
+      <c r="E31" s="11">
         <v>4514</v>
       </c>
-      <c r="F31" s="12">
+      <c r="F31" s="11">
         <v>2098</v>
       </c>
-      <c r="G31" s="12">
+      <c r="G31" s="11">
         <v>2392</v>
       </c>
-      <c r="H31" s="12">
+      <c r="H31" s="11">
         <v>4329</v>
       </c>
-      <c r="I31" s="12">
+      <c r="I31" s="11">
         <v>232</v>
       </c>
-      <c r="J31" s="16">
+      <c r="J31" s="15">
         <v>3459</v>
       </c>
-      <c r="K31" s="17">
+      <c r="K31" s="16">
         <v>785</v>
       </c>
-      <c r="L31" s="17">
+      <c r="L31" s="16">
         <v>610</v>
       </c>
-      <c r="M31" s="17">
+      <c r="M31" s="16">
         <v>5161</v>
       </c>
-      <c r="N31" s="17">
+      <c r="N31" s="16">
         <v>2222</v>
       </c>
-      <c r="O31" s="17">
+      <c r="O31" s="16">
         <v>2309</v>
       </c>
-      <c r="P31" s="17">
+      <c r="P31" s="16">
         <v>5019</v>
       </c>
-      <c r="Q31" s="17">
+      <c r="Q31" s="16">
         <v>311</v>
       </c>
-      <c r="R31" s="11">
+      <c r="R31" s="10">
         <v>2704</v>
       </c>
-      <c r="S31" s="12">
+      <c r="S31" s="11">
         <v>796</v>
       </c>
-      <c r="T31" s="12">
+      <c r="T31" s="11">
         <v>866</v>
       </c>
-      <c r="U31" s="12">
+      <c r="U31" s="11">
         <v>2042</v>
       </c>
-      <c r="V31" s="12">
+      <c r="V31" s="11">
         <v>2048</v>
       </c>
-      <c r="W31" s="12">
+      <c r="W31" s="11">
         <v>2238</v>
       </c>
-      <c r="X31" s="12">
+      <c r="X31" s="11">
         <v>4622</v>
       </c>
-      <c r="Y31" s="12">
+      <c r="Y31" s="11">
         <v>242</v>
       </c>
     </row>
     <row r="34" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B34" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="5"/>
-      <c r="J34" s="5"/>
-      <c r="K34" s="5"/>
       <c r="R34" s="5"/>
       <c r="S34" s="5"/>
     </row>
     <row r="35" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B35" t="s">
-        <v>1</v>
-      </c>
-      <c r="C35" t="s">
-        <v>2</v>
-      </c>
-      <c r="D35" t="s">
-        <v>3</v>
-      </c>
-      <c r="E35" t="s">
-        <v>4</v>
-      </c>
-      <c r="F35" t="s">
-        <v>5</v>
-      </c>
-      <c r="G35" t="s">
-        <v>6</v>
-      </c>
-      <c r="H35" t="s">
-        <v>7</v>
-      </c>
-      <c r="I35" t="s">
-        <v>8</v>
-      </c>
-      <c r="J35" t="s">
-        <v>9</v>
-      </c>
-      <c r="K35" t="s">
-        <v>10</v>
-      </c>
-      <c r="L35" t="s">
-        <v>11</v>
-      </c>
-      <c r="M35" t="s">
-        <v>12</v>
-      </c>
-      <c r="N35" t="s">
-        <v>13</v>
-      </c>
-      <c r="O35" t="s">
-        <v>14</v>
-      </c>
-      <c r="P35" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q35" t="s">
-        <v>16</v>
-      </c>
-      <c r="R35" s="7"/>
-      <c r="S35" s="7"/>
+      <c r="R35" s="6"/>
+      <c r="S35" s="6"/>
     </row>
     <row r="36" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B36" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="J36" s="7"/>
-      <c r="K36" s="7"/>
-      <c r="Q36" s="7"/>
-      <c r="R36" s="7"/>
-      <c r="S36" s="7"/>
+      <c r="S36" s="6"/>
     </row>
     <row r="37" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B37">
-        <f xml:space="preserve"> MEDIAN(B16, B30, J28, R24, R30)</f>
-        <v>151</v>
-      </c>
-      <c r="R37" s="7"/>
-      <c r="S37" s="7"/>
+      <c r="S37" s="6"/>
     </row>
     <row r="38" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B38" s="6"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
-      <c r="I38" s="7"/>
-      <c r="J38" s="7"/>
-      <c r="K38" s="7"/>
-      <c r="Q38" s="7"/>
-      <c r="R38" s="7"/>
-      <c r="S38" s="7"/>
+      <c r="S38" s="6"/>
     </row>
     <row r="39" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B39" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="I39" s="32" t="s">
-        <v>2</v>
-      </c>
-      <c r="J39" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="K39" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="L39" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="M39" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="N39" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="O39" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q39" s="7"/>
-      <c r="R39" s="7"/>
-      <c r="S39" s="7"/>
+      <c r="S39" s="6"/>
     </row>
     <row r="40" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B40" s="6">
-        <f xml:space="preserve"> MEDIAN(B28, J20, R18, R20, R28)</f>
-        <v>164</v>
-      </c>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="I40" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="J40" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="K40" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="L40" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="M40" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="N40" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="O40" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="P40" s="6"/>
-      <c r="Q40" s="6"/>
-      <c r="R40" s="7"/>
-      <c r="S40" s="7"/>
+      <c r="S40" s="6"/>
     </row>
     <row r="41" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B41" s="6"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="7"/>
-      <c r="I41" s="7"/>
-      <c r="J41" s="7"/>
-      <c r="K41" s="7"/>
-      <c r="L41" s="7"/>
-      <c r="Q41" s="7"/>
-      <c r="R41" s="7"/>
-      <c r="S41" s="7"/>
-    </row>
-    <row r="42" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B42" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="7"/>
-      <c r="I42" s="7"/>
-      <c r="J42" s="7"/>
-      <c r="K42" s="7"/>
-      <c r="L42" s="7"/>
-      <c r="Q42" s="7"/>
-      <c r="R42" s="7"/>
-    </row>
-    <row r="43" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B43" s="7">
-        <f xml:space="preserve"> MEDIAN(B18, B20, B22, B26, J30)</f>
-        <v>164</v>
-      </c>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="7"/>
-      <c r="I43" s="7"/>
-      <c r="J43" s="7"/>
-      <c r="K43" s="7"/>
-      <c r="L43" s="7"/>
-      <c r="M43" s="7"/>
-      <c r="N43" s="7"/>
-      <c r="O43" s="7"/>
-      <c r="P43" s="7"/>
-      <c r="Q43" s="7"/>
-      <c r="R43" s="7"/>
-    </row>
-    <row r="44" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B44" s="7"/>
-      <c r="C44" s="7"/>
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
-      <c r="G44" s="7"/>
-      <c r="K44" s="7"/>
-      <c r="L44" s="7"/>
-    </row>
-    <row r="45" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B45" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="K45" s="7"/>
-      <c r="L45" s="7"/>
-    </row>
-    <row r="46" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B46">
-        <f xml:space="preserve"> MEDIAN(B24, J18, J22, J26, R16)</f>
-        <v>166</v>
-      </c>
+      <c r="S41" s="6"/>
     </row>
     <row r="48" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B48" s="29" t="s">
-        <v>60</v>
+      <c r="B48" s="27" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="49" spans="2:19" x14ac:dyDescent="0.2">
@@ -2419,7 +2175,7 @@
         <v>140.5</v>
       </c>
       <c r="E50">
-        <f t="shared" ref="E50:H50" si="0" xml:space="preserve"> MEDIAN(M16, M24, U22, U26)</f>
+        <f t="shared" ref="E50:G50" si="0" xml:space="preserve"> MEDIAN(M16, M24, U22, U26)</f>
         <v>424</v>
       </c>
       <c r="F50">
@@ -2472,8 +2228,8 @@
       </c>
     </row>
     <row r="53" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B53" s="29" t="s">
-        <v>61</v>
+      <c r="B53" s="27" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="2:19" x14ac:dyDescent="0.2">
@@ -2521,129 +2277,129 @@
       </c>
     </row>
     <row r="55" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B55" s="10" t="s">
+      <c r="B55" s="9" t="s">
         <v>18</v>
       </c>
       <c r="C55">
         <v>1</v>
       </c>
       <c r="D55">
-        <f xml:space="preserve"> (C16 - $B$37) / (C50 - $B$37)</f>
-        <v>0.69471683770429493</v>
+        <f xml:space="preserve"> (C16 - B50) / (C50 - B50)</f>
+        <v>0.69546919431279619</v>
       </c>
       <c r="E55">
-        <f xml:space="preserve"> (E16 - $B$37) / (E50 - $B$37)</f>
-        <v>0.82051282051282048</v>
+        <f xml:space="preserve"> (E16 - B50) / (E50 - B50)</f>
+        <v>0.83960720130932898</v>
       </c>
       <c r="F55">
-        <f t="shared" ref="F55:H55" si="2" xml:space="preserve"> (F16 - $B$37) / (F50 - $B$37)</f>
-        <v>0.74264972776769511</v>
+        <f xml:space="preserve"> (F16 - B50) / (F50 - B50)</f>
+        <v>0.74332260659694283</v>
       </c>
       <c r="G55">
-        <f t="shared" si="2"/>
-        <v>0.62919964278015583</v>
+        <f xml:space="preserve"> (G16 - B50) / (G50 - B50)</f>
+        <v>0.6299403774048804</v>
       </c>
       <c r="H55">
-        <f t="shared" si="2"/>
-        <v>0.70902281832433378</v>
+        <f xml:space="preserve"> (H16 - B50) / (H50 - B50)</f>
+        <v>0.70984410960093791</v>
       </c>
       <c r="I55">
-        <f xml:space="preserve"> (I16 - $B$37) / (I50 - $B$37)</f>
-        <v>0.67287646928365497</v>
+        <f xml:space="preserve"> (I16 - B50) / (I50 - B50)</f>
+        <v>0.67752514210756454</v>
       </c>
       <c r="J55">
-        <f xml:space="preserve"> (B17 - $B$37) / (J50 - $B$37)</f>
-        <v>0.41729284611425632</v>
+        <f xml:space="preserve"> (B17 - B50) / (J50 - B50)</f>
+        <v>0.42116564417177915</v>
       </c>
       <c r="K55">
-        <f t="shared" ref="K55:Q55" si="3" xml:space="preserve"> (C17 - $B$37) / (K50 - $B$37)</f>
-        <v>0.4108563406644829</v>
+        <f xml:space="preserve"> (C17 - B50) / (K50 - B50)</f>
+        <v>0.42824704813805631</v>
       </c>
       <c r="L55">
-        <f xml:space="preserve"> (D17 - $B$37) / (L50 - $B$37)</f>
-        <v>0.4009171306911235</v>
+        <f xml:space="preserve"> (D17 - B50) / (L50 - B50)</f>
+        <v>0.41340602950609368</v>
       </c>
       <c r="M55">
-        <f t="shared" si="3"/>
-        <v>0.55381990023628247</v>
+        <f xml:space="preserve"> (E17 - B50) / (M50 - B50)</f>
+        <v>0.55571531272465857</v>
       </c>
       <c r="N55">
-        <f t="shared" si="3"/>
-        <v>0.24364020351348756</v>
+        <f xml:space="preserve"> (F17 - B50) / (N50 - B50)</f>
+        <v>0.2483304712841061</v>
       </c>
       <c r="O55">
-        <f t="shared" si="3"/>
-        <v>0.18682399213372664</v>
+        <f xml:space="preserve"> (G17 - B50) / (O50 - B50)</f>
+        <v>0.19051947143955814</v>
       </c>
       <c r="P55">
-        <f xml:space="preserve"> (H17 - $B$37) / (P50 - $B$37)</f>
-        <v>0.35471942313025795</v>
+        <f xml:space="preserve"> (H17 - B50) / (P50 - B50)</f>
+        <v>0.35665238029402274</v>
       </c>
       <c r="Q55">
-        <f xml:space="preserve"> (I17 - $B$37) / (Q50 - $B$37)</f>
-        <v>0.31818181818181818</v>
-      </c>
-      <c r="S55" s="7"/>
+        <f xml:space="preserve"> (I17 - B50) / (Q50 - B50)</f>
+        <v>0.39890710382513661</v>
+      </c>
+      <c r="S55" s="6"/>
     </row>
     <row r="56" spans="2:19" x14ac:dyDescent="0.2">
       <c r="C56">
         <v>2</v>
       </c>
       <c r="D56">
-        <f xml:space="preserve"> (C30 - $B$37) / (C50 - $B$37)</f>
-        <v>0.85077917141771187</v>
+        <f xml:space="preserve"> (C30 - B50) / (C50 - B50)</f>
+        <v>0.85114691943127962</v>
       </c>
       <c r="E56">
-        <f xml:space="preserve"> (E30 - $B$37) / (E50 - $B$37)</f>
-        <v>0.89010989010989006</v>
+        <f xml:space="preserve"> (E30 - B50) / (E50 - B50)</f>
+        <v>0.90180032733224225</v>
       </c>
       <c r="F56">
-        <f t="shared" ref="F56:H56" si="4" xml:space="preserve"> (F30 - $B$37) / (F50 - $B$37)</f>
-        <v>0.87953216374269005</v>
+        <f xml:space="preserve"> (F30 - B50) / (F50 - B50)</f>
+        <v>0.87984714400643604</v>
       </c>
       <c r="G56">
-        <f t="shared" si="4"/>
-        <v>0.74523450250977741</v>
+        <f xml:space="preserve"> (G30 - B50) / (G50 - B50)</f>
+        <v>0.74574343844120716</v>
       </c>
       <c r="H56">
-        <f t="shared" si="4"/>
-        <v>0.75126284619404282</v>
+        <f xml:space="preserve"> (H30 - B50) / (H50 - B50)</f>
+        <v>0.75196491380433361</v>
       </c>
       <c r="I56">
-        <f xml:space="preserve"> (I30 - $B$37) / (I50 - $B$37)</f>
-        <v>0.70037702373031718</v>
+        <f xml:space="preserve"> (I30 - B50) / (I50 - B50)</f>
+        <v>0.70463489287275904</v>
       </c>
       <c r="J56">
-        <f xml:space="preserve"> (B31 - $B$37) / (J50 - $B$37)</f>
-        <v>0.53113741636644363</v>
+        <f xml:space="preserve"> (B31 - B50) / (J50 - B50)</f>
+        <v>0.53425357873210633</v>
       </c>
       <c r="K56">
-        <f t="shared" ref="K56:Q56" si="5" xml:space="preserve"> (C31 - $B$37) / (K50 - $B$37)</f>
-        <v>0.52784277023865234</v>
+        <f xml:space="preserve"> (C31 - B50) / (K50 - B50)</f>
+        <v>0.54178019981834691</v>
       </c>
       <c r="L56">
-        <f xml:space="preserve"> (D31 - $B$37) / (L50 - $B$37)</f>
-        <v>0.429741238126433</v>
+        <f xml:space="preserve"> (D31 - B50) / (L50 - B50)</f>
+        <v>0.44162924951892241</v>
       </c>
       <c r="M56">
-        <f t="shared" si="5"/>
-        <v>0.57272249934365971</v>
+        <f xml:space="preserve"> (E31 - B50) / (M50 - B50)</f>
+        <v>0.57453761192078945</v>
       </c>
       <c r="N56">
-        <f t="shared" si="5"/>
-        <v>0.37381203801478352</v>
+        <f xml:space="preserve"> (F31 - B50) / (N50 - B50)</f>
+        <v>0.37769509635565734</v>
       </c>
       <c r="O56">
-        <f t="shared" si="5"/>
-        <v>0.31479140328697852</v>
+        <f xml:space="preserve"> (G31 - B50) / (O50 - B50)</f>
+        <v>0.31790533454520031</v>
       </c>
       <c r="P56">
-        <f t="shared" si="5"/>
-        <v>0.38624387538134419</v>
+        <f xml:space="preserve"> (H31 - B50) / (P50 - B50)</f>
+        <v>0.38808240011060419</v>
       </c>
       <c r="Q56">
-        <f t="shared" si="5"/>
-        <v>0.33471074380165289</v>
+        <f xml:space="preserve"> (I31 - B50) / (Q50 - B50)</f>
+        <v>0.4134790528233151</v>
       </c>
     </row>
     <row r="57" spans="2:19" x14ac:dyDescent="0.2">
@@ -2651,60 +2407,60 @@
         <v>3</v>
       </c>
       <c r="D57">
-        <f xml:space="preserve"> (K28 - $B$37) / (C50 - $B$37)</f>
-        <v>0.86621056632459137</v>
+        <f xml:space="preserve"> (K28 - B50) / (C50 - B50)</f>
+        <v>0.86654028436018959</v>
       </c>
       <c r="E57">
-        <f xml:space="preserve"> (M28 - $B$37) / (E50 - $B$37)</f>
-        <v>0.91208791208791207</v>
+        <f xml:space="preserve"> (M28 - B50) / (E50 - B50)</f>
+        <v>0.92144026186579375</v>
       </c>
       <c r="F57">
-        <f t="shared" ref="F57:I57" si="6" xml:space="preserve"> (N28 - $B$37) / (F50 - $B$37)</f>
-        <v>0.89832627545876187</v>
+        <f xml:space="preserve"> (N28 - B50) / (F50 - B50)</f>
+        <v>0.89859211584875298</v>
       </c>
       <c r="G57">
-        <f t="shared" si="6"/>
-        <v>0.7675915375850707</v>
+        <f xml:space="preserve"> (O28 - B50) / (G50 - B50)</f>
+        <v>0.76805581166635928</v>
       </c>
       <c r="H57">
-        <f t="shared" si="6"/>
-        <v>0.75396272426406552</v>
+        <f xml:space="preserve"> (P28 - B50) / (H50 - B50)</f>
+        <v>0.75465717139259192</v>
       </c>
       <c r="I57">
-        <f t="shared" si="6"/>
-        <v>0.70126413838988688</v>
+        <f xml:space="preserve"> (Q28 - B50) / (I50 - B50)</f>
+        <v>0.70550940096195891</v>
       </c>
       <c r="J57">
-        <f xml:space="preserve"> (J29 - $B$37) / (J50 - $B$37)</f>
-        <v>0.51013896037056095</v>
+        <f xml:space="preserve"> (J29 - B50) / (J50 - B50)</f>
+        <v>0.51339468302658486</v>
       </c>
       <c r="K57">
-        <f t="shared" ref="K57:Q57" si="7" xml:space="preserve"> (K29 - $B$37) / (K50 - $B$37)</f>
-        <v>0.57463734206832007</v>
+        <f xml:space="preserve"> (K29 - B50) / (K50 - B50)</f>
+        <v>0.58719346049046317</v>
       </c>
       <c r="L57">
-        <f xml:space="preserve"> (L29 - $B$37) / (L50 - $B$37)</f>
-        <v>0.43760235833606287</v>
+        <f xml:space="preserve"> (L29 - B50) / (L50 - B50)</f>
+        <v>0.44932649134060293</v>
       </c>
       <c r="M57">
-        <f t="shared" si="7"/>
-        <v>0.58860593331583089</v>
+        <f xml:space="preserve"> (M29 - B50) / (M50 - B50)</f>
+        <v>0.59035357166198288</v>
       </c>
       <c r="N57">
-        <f t="shared" si="7"/>
-        <v>0.38840357108572526</v>
+        <f xml:space="preserve"> (N29 - B50) / (N50 - B50)</f>
+        <v>0.39219614577370732</v>
       </c>
       <c r="O57">
-        <f t="shared" si="7"/>
-        <v>0.30832982160415789</v>
+        <f xml:space="preserve"> (O29 - B50) / (O50 - B50)</f>
+        <v>0.31147311752779139</v>
       </c>
       <c r="P57">
-        <f t="shared" si="7"/>
-        <v>0.4012203013774614</v>
+        <f xml:space="preserve"> (P29 - B50) / (P50 - B50)</f>
+        <v>0.40301396377713261</v>
       </c>
       <c r="Q57">
-        <f t="shared" si="7"/>
-        <v>0.36363636363636365</v>
+        <f xml:space="preserve"> (Q29 - B50) / (Q50 - B50)</f>
+        <v>0.43897996357012753</v>
       </c>
     </row>
     <row r="58" spans="2:19" x14ac:dyDescent="0.2">
@@ -2712,60 +2468,60 @@
         <v>4</v>
       </c>
       <c r="D58">
-        <f xml:space="preserve"> (S24 - $B$37) / (C50 - $B$37)</f>
-        <v>0.87153173698213604</v>
+        <f xml:space="preserve"> (S24 - B50) / (C50 - B50)</f>
+        <v>0.87184834123222754</v>
       </c>
       <c r="E58">
-        <f xml:space="preserve"> (U24 - $B$37) / (E50 - $B$37)</f>
-        <v>0.87912087912087911</v>
+        <f xml:space="preserve"> (U24 - B50) / (E50 - B50)</f>
+        <v>0.89198036006546644</v>
       </c>
       <c r="F58">
-        <f t="shared" ref="F58:I58" si="8" xml:space="preserve"> (V24 - $B$37) / (F50 - $B$37)</f>
-        <v>0.89082476305706793</v>
+        <f xml:space="preserve"> (V24 - B50) / (F50 - B50)</f>
+        <v>0.89111021721641193</v>
       </c>
       <c r="G58">
-        <f t="shared" si="8"/>
-        <v>0.76020078218827947</v>
+        <f xml:space="preserve"> (W24 - B50) / (G50 - B50)</f>
+        <v>0.76067982051754868</v>
       </c>
       <c r="H58">
-        <f t="shared" si="8"/>
-        <v>0.73131858561226271</v>
+        <f xml:space="preserve"> (X24 - B50) / (H50 - B50)</f>
+        <v>0.73207694645881283</v>
       </c>
       <c r="I58">
-        <f t="shared" si="8"/>
-        <v>0.62763362164559766</v>
+        <f xml:space="preserve"> (Y24 - B50) / (I50 - B50)</f>
+        <v>0.63292522955837338</v>
       </c>
       <c r="J58">
-        <f xml:space="preserve"> (R25 - $B$37) / (J50 - $B$37)</f>
-        <v>0.4901698404529079</v>
+        <f xml:space="preserve"> (R25 - B50) / (J50 - B50)</f>
+        <v>0.49355828220858894</v>
       </c>
       <c r="K58">
-        <f t="shared" ref="K58:Q58" si="9" xml:space="preserve"> (S25 - $B$37) / (K50 - $B$37)</f>
-        <v>0.55124005615348615</v>
+        <f xml:space="preserve"> (S25 - B50) / (K50 - B50)</f>
+        <v>0.56448683015440504</v>
       </c>
       <c r="L58">
-        <f xml:space="preserve"> (T25 - $B$37) / (L50 - $B$37)</f>
-        <v>0.43105142482803799</v>
+        <f xml:space="preserve"> (T25 - B50) / (L50 - B50)</f>
+        <v>0.44291212315586914</v>
       </c>
       <c r="M58">
-        <f t="shared" si="9"/>
-        <v>0.57219742714623256</v>
+        <f xml:space="preserve"> (U25 - B50) / (M50 - B50)</f>
+        <v>0.57401477027645254</v>
       </c>
       <c r="N58">
-        <f t="shared" si="9"/>
-        <v>0.38091581069405778</v>
+        <f xml:space="preserve"> (V25 - B50) / (N50 - B50)</f>
+        <v>0.38475481778286585</v>
       </c>
       <c r="O58">
-        <f t="shared" si="9"/>
-        <v>0.31198201994662172</v>
+        <f xml:space="preserve"> (W25 - B50) / (O50 - B50)</f>
+        <v>0.31510871845067467</v>
       </c>
       <c r="P58">
-        <f t="shared" si="9"/>
-        <v>0.37949523897568643</v>
+        <f xml:space="preserve"> (X25 - B50) / (P50 - B50)</f>
+        <v>0.38135397944605742</v>
       </c>
       <c r="Q58">
-        <f t="shared" si="9"/>
-        <v>0.33471074380165289</v>
+        <f xml:space="preserve"> (Y25 - B50) / (Q50 - B50)</f>
+        <v>0.4134790528233151</v>
       </c>
     </row>
     <row r="59" spans="2:19" x14ac:dyDescent="0.2">
@@ -2773,124 +2529,124 @@
         <v>5</v>
       </c>
       <c r="D59">
-        <f xml:space="preserve"> (S30 - $B$37) / (C50 - $B$37)</f>
-        <v>0.88430254656024321</v>
+        <f xml:space="preserve"> (S30 - B50) / (C50 - B50)</f>
+        <v>0.88458767772511848</v>
       </c>
       <c r="E59">
-        <f xml:space="preserve"> (U30 - $B$37) / (E50 - $B$37)</f>
-        <v>0.94505494505494503</v>
+        <f xml:space="preserve"> (U30 - B50) / (E50 - B50)</f>
+        <v>0.95090016366612107</v>
       </c>
       <c r="F59">
-        <f t="shared" ref="F59:I59" si="10" xml:space="preserve"> (V30 - $B$37) / (F50 - $B$37)</f>
-        <v>0.87848356523492643</v>
+        <f xml:space="preserve"> (V30 - B50) / (F50 - B50)</f>
+        <v>0.87880128720836681</v>
       </c>
       <c r="G59">
-        <f t="shared" si="10"/>
-        <v>0.77953992547654971</v>
+        <f xml:space="preserve"> (W30 - B50) / (G50 - B50)</f>
+        <v>0.77998033069026984</v>
       </c>
       <c r="H59">
-        <f t="shared" si="10"/>
-        <v>0.78984497474307613</v>
+        <f xml:space="preserve"> (X30 - B50) / (H50 - B50)</f>
+        <v>0.79043814321073425</v>
       </c>
       <c r="I59">
-        <f t="shared" si="10"/>
-        <v>0.69328010645375915</v>
+        <f xml:space="preserve"> (Y30 - B50) / (I50 - B50)</f>
+        <v>0.69763882815916045</v>
       </c>
       <c r="J59">
-        <f xml:space="preserve"> (R31 - $B$37) / (J50 - $B$37)</f>
-        <v>0.52557900154400417</v>
+        <f xml:space="preserve"> (R31 - B50) / (J50 - B50)</f>
+        <v>0.52873210633946832</v>
       </c>
       <c r="K59">
-        <f t="shared" ref="K59:Q59" si="11" xml:space="preserve"> (S31 - $B$37) / (K50 - $B$37)</f>
-        <v>0.60364997660271413</v>
+        <f xml:space="preserve"> (S31 - B50) / (K50 - B50)</f>
+        <v>0.61534968210717533</v>
       </c>
       <c r="L59">
-        <f xml:space="preserve"> (T31 - $B$37) / (L50 - $B$37)</f>
-        <v>0.4683917458237799</v>
+        <f xml:space="preserve"> (T31 - B50) / (L50 - B50)</f>
+        <v>0.47947402180885185</v>
       </c>
       <c r="M59">
-        <f t="shared" si="11"/>
-        <v>0.24822788133368337</v>
+        <f xml:space="preserve"> (U31 - B50) / (M50 - B50)</f>
+        <v>0.25142147572054113</v>
       </c>
       <c r="N59">
-        <f t="shared" si="11"/>
-        <v>0.36421234520495344</v>
+        <f xml:space="preserve"> (V31 - B50) / (N50 - B50)</f>
+        <v>0.36815493226483498</v>
       </c>
       <c r="O59">
-        <f t="shared" si="11"/>
-        <v>0.29315915156623124</v>
+        <f xml:space="preserve"> (W31 - B50) / (O50 - B50)</f>
+        <v>0.29637139061735301</v>
       </c>
       <c r="P59">
-        <f t="shared" si="11"/>
-        <v>0.41333086807802533</v>
+        <f xml:space="preserve"> (X31 - B50) / (P50 - B50)</f>
+        <v>0.41508825291488088</v>
       </c>
       <c r="Q59">
-        <f t="shared" si="11"/>
-        <v>0.37603305785123969</v>
+        <f xml:space="preserve"> (Y31 - B50) / (Q50 - B50)</f>
+        <v>0.44990892531876137</v>
       </c>
     </row>
     <row r="61" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B61" s="31" t="s">
+      <c r="B61" s="29" t="s">
         <v>20</v>
       </c>
       <c r="C61">
         <v>1</v>
       </c>
       <c r="D61">
-        <f xml:space="preserve"> (C28 - $B$40) / (C50 - $B$40)</f>
-        <v>0.54968802313194343</v>
+        <f xml:space="preserve"> (C28 - B50) / (C50 - B50)</f>
+        <v>0.55124170616113743</v>
       </c>
       <c r="E61">
-        <f xml:space="preserve"> (E28 - $B$40) / (E50 - $B$40)</f>
-        <v>0.50384615384615383</v>
+        <f xml:space="preserve"> (E28 - B50) / (E50 - B50)</f>
+        <v>0.57774140752864156</v>
       </c>
       <c r="F61">
-        <f t="shared" ref="F61:I61" si="12" xml:space="preserve"> (F28 - $B$40) / (F50 - $B$40)</f>
-        <v>0.49142072752230609</v>
+        <f xml:space="preserve"> (F28 - B50) / (F50 - B50)</f>
+        <v>0.49328238133547869</v>
       </c>
       <c r="G61">
-        <f t="shared" si="12"/>
-        <v>0.44429377138102139</v>
+        <f xml:space="preserve"> (G28 - B50) / (G50 - B50)</f>
+        <v>0.44584793164914871</v>
       </c>
       <c r="H61">
-        <f xml:space="preserve"> (H28 - $B$40) / (H50 - $B$40)</f>
-        <v>0.53012468393059553</v>
+        <f xml:space="preserve"> (H28 - B50) / (H50 - B50)</f>
+        <v>0.53198141473793914</v>
       </c>
       <c r="I61">
-        <f xml:space="preserve"> (I28 - $B$40) / (I50 - $B$40)</f>
-        <v>0.56435422708008032</v>
+        <f xml:space="preserve"> (I28 - B50) / (I50 - B50)</f>
+        <v>0.57302142544818535</v>
       </c>
       <c r="J61">
-        <f xml:space="preserve"> (B29 - $B$40) / (J50 - $B$40)</f>
-        <v>0.49210444834348233</v>
+        <f xml:space="preserve"> (B29 - B50) / (J50 - B50)</f>
+        <v>0.49683026584867074</v>
       </c>
       <c r="K61">
-        <f t="shared" ref="K61:Q61" si="13" xml:space="preserve"> (C29 - $B$40) / (K50 - $B$40)</f>
-        <v>0.50023685457129319</v>
+        <f xml:space="preserve"> (C29 - B50) / (K50 - B50)</f>
+        <v>0.52089009990917345</v>
       </c>
       <c r="L61">
-        <f t="shared" si="13"/>
-        <v>0.17509084902543773</v>
+        <f xml:space="preserve"> (D29 - B50) / (L50 - B50)</f>
+        <v>0.19916613213598461</v>
       </c>
       <c r="M61">
-        <f t="shared" si="13"/>
-        <v>0.19526627218934911</v>
+        <f xml:space="preserve"> (E29 - B50) / (M50 - B50)</f>
+        <v>0.20005228416443369</v>
       </c>
       <c r="N61">
-        <f t="shared" si="13"/>
-        <v>0.27004138196516214</v>
+        <f xml:space="preserve"> (F29 - B50) / (N50 - B50)</f>
+        <v>0.27637855371112385</v>
       </c>
       <c r="O61">
-        <f t="shared" si="13"/>
-        <v>0.4126090627638615</v>
+        <f xml:space="preserve"> (G29 - B50) / (O50 - B50)</f>
+        <v>0.4163462210725023</v>
       </c>
       <c r="P61">
-        <f t="shared" si="13"/>
-        <v>0.20705294335431321</v>
+        <f xml:space="preserve"> (H29 - B50) / (P50 - B50)</f>
+        <v>0.21037835844969816</v>
       </c>
       <c r="Q61">
-        <f t="shared" si="13"/>
-        <v>7.8602620087336247E-2</v>
+        <f xml:space="preserve"> (I29 - B50) / (Q50 - B50)</f>
+        <v>0.23132969034608378</v>
       </c>
     </row>
     <row r="62" spans="2:19" x14ac:dyDescent="0.2">
@@ -2898,60 +2654,60 @@
         <v>2</v>
       </c>
       <c r="D62">
-        <f xml:space="preserve"> (K20 - $B$40) / (C50 - $B$40)</f>
-        <v>0.55577537665499921</v>
+        <f xml:space="preserve"> (K20 - B50) / (C50 - B50)</f>
+        <v>0.55730805687203788</v>
       </c>
       <c r="E62">
-        <f xml:space="preserve"> (M20 - $B$40) / (E50 - $B$40)</f>
-        <v>0.45769230769230768</v>
+        <f xml:space="preserve"> (M20 - B50) / (E50 - B50)</f>
+        <v>0.53846153846153844</v>
       </c>
       <c r="F62">
-        <f t="shared" ref="F62:I62" si="14" xml:space="preserve"> (N20 - $B$40) / (F50 - $B$40)</f>
-        <v>0.49683071581412247</v>
+        <f xml:space="preserve"> (N20 - B50) / (F50 - B50)</f>
+        <v>0.49867256637168139</v>
       </c>
       <c r="G62">
-        <f t="shared" si="14"/>
-        <v>0.44078034949301936</v>
+        <f xml:space="preserve"> (O20 - B50) / (G50 - B50)</f>
+        <v>0.44234433585346367</v>
       </c>
       <c r="H62">
-        <f xml:space="preserve"> (P20 - $B$40) / (H50 - $B$40)</f>
-        <v>0.53265323916644869</v>
+        <f xml:space="preserve"> (P20 - B50) / (H50 - B50)</f>
+        <v>0.53449997828824525</v>
       </c>
       <c r="I62">
-        <f xml:space="preserve"> (Q20 - $B$40) / (I50 - $B$40)</f>
-        <v>0.51751059558331469</v>
+        <f xml:space="preserve"> (Q20 - B50) / (I50 - B50)</f>
+        <v>0.52710975076519462</v>
       </c>
       <c r="J62">
-        <f xml:space="preserve"> (J21 - $B$40) / (J50 - $B$40)</f>
-        <v>0.49231086799463308</v>
+        <f xml:space="preserve"> (J21 - B50) / (J50 - B50)</f>
+        <v>0.49703476482617587</v>
       </c>
       <c r="K62">
-        <f t="shared" ref="K62:Q62" si="15" xml:space="preserve"> (K21 - $B$40) / (K50 - $B$40)</f>
-        <v>0.4007579346281383</v>
+        <f xml:space="preserve"> (K21 - B50) / (K50 - B50)</f>
+        <v>0.42552225249772935</v>
       </c>
       <c r="L62">
-        <f t="shared" si="15"/>
-        <v>0.17773372976544433</v>
+        <f xml:space="preserve"> (L21 - B50) / (L50 - B50)</f>
+        <v>0.20173187940987813</v>
       </c>
       <c r="M62">
-        <f t="shared" si="15"/>
-        <v>0.19881656804733727</v>
+        <f xml:space="preserve"> (M21 - B50) / (M50 - B50)</f>
+        <v>0.20358146526370827</v>
       </c>
       <c r="N62">
-        <f t="shared" si="15"/>
-        <v>0.25310364738716196</v>
+        <f xml:space="preserve"> (N21 - B50) / (N50 - B50)</f>
+        <v>0.2595878649112765</v>
       </c>
       <c r="O62">
-        <f t="shared" si="15"/>
-        <v>0.44962003940332113</v>
+        <f xml:space="preserve"> (O21 - B50) / (O50 - B50)</f>
+        <v>0.45312172271551421</v>
       </c>
       <c r="P62">
-        <f t="shared" si="15"/>
-        <v>0.20973713439466865</v>
+        <f xml:space="preserve"> (P21 - B50) / (P50 - B50)</f>
+        <v>0.21305129268629891</v>
       </c>
       <c r="Q62">
-        <f t="shared" si="15"/>
-        <v>6.9868995633187769E-2</v>
+        <f xml:space="preserve"> (Q21 - B50) / (Q50 - B50)</f>
+        <v>0.22404371584699453</v>
       </c>
     </row>
     <row r="63" spans="2:19" x14ac:dyDescent="0.2">
@@ -2959,60 +2715,60 @@
         <v>3</v>
       </c>
       <c r="D63">
-        <f xml:space="preserve"> (S18 - $B$40) / (C50 - $B$40)</f>
-        <v>0.3980368284888145</v>
+        <f xml:space="preserve"> (S18 - B50) / (C50 - B50)</f>
+        <v>0.40011374407582939</v>
       </c>
       <c r="E63">
-        <f xml:space="preserve"> (U18 - $B$40) / (E50 - $B$40)</f>
-        <v>0.31153846153846154</v>
+        <f xml:space="preserve"> (U18 - B50) / (E50 - B50)</f>
+        <v>0.41407528641571195</v>
       </c>
       <c r="F63">
-        <f t="shared" ref="F63:I63" si="16" xml:space="preserve"> (V18 - $B$40) / (F50 - $B$40)</f>
-        <v>0.39145706326456459</v>
+        <f xml:space="preserve"> (V18 - B50) / (F50 - B50)</f>
+        <v>0.39368463395012065</v>
       </c>
       <c r="G63">
-        <f t="shared" si="16"/>
-        <v>0.32378956452060281</v>
+        <f xml:space="preserve"> (W18 - B50) / (G50 - B50)</f>
+        <v>0.3256807425164423</v>
       </c>
       <c r="H63">
-        <f xml:space="preserve"> (X18 - $B$40) / (H50 - $B$40)</f>
-        <v>0.51460458627604844</v>
+        <f xml:space="preserve"> (X18 - B50) / (H50 - B50)</f>
+        <v>0.51652264536019799</v>
       </c>
       <c r="I63">
-        <f xml:space="preserve"> (Y18 - $B$40) / (I50 - $B$40)</f>
-        <v>0.50992638857907646</v>
+        <f xml:space="preserve"> (Y18 - B50) / (I50 - B50)</f>
+        <v>0.51967643200699609</v>
       </c>
       <c r="J63">
-        <f xml:space="preserve"> (R19 - $B$40) / (J50 - $B$40)</f>
-        <v>0.38889462276808751</v>
+        <f xml:space="preserve"> (R19 - B50) / (J50 - B50)</f>
+        <v>0.3945807770961145</v>
       </c>
       <c r="K63">
-        <f t="shared" ref="K63:Q63" si="17" xml:space="preserve"> (S19 - $B$40) / (K50 - $B$40)</f>
-        <v>0.25864519185220275</v>
+        <f xml:space="preserve"> (S19 - B50) / (K50 - B50)</f>
+        <v>0.28928247048138056</v>
       </c>
       <c r="L63">
-        <f t="shared" si="17"/>
-        <v>0.1275189957053188</v>
+        <f xml:space="preserve"> (T19 - B50) / (L50 - B50)</f>
+        <v>0.15298268120590122</v>
       </c>
       <c r="M63">
-        <f t="shared" si="17"/>
-        <v>0.14122287968441816</v>
+        <f xml:space="preserve"> (U19 - B50) / (M50 - B50)</f>
+        <v>0.14633030520880988</v>
       </c>
       <c r="N63">
-        <f t="shared" si="17"/>
-        <v>0.13184486574920604</v>
+        <f xml:space="preserve"> (V19 - B50) / (N50 - B50)</f>
+        <v>0.13938179736691472</v>
       </c>
       <c r="O63">
-        <f t="shared" si="17"/>
-        <v>0.22783563186039965</v>
+        <f xml:space="preserve"> (W19 - B50) / (O50 - B50)</f>
+        <v>0.23274837446689506</v>
       </c>
       <c r="P63">
-        <f t="shared" si="17"/>
-        <v>0.21094039244724178</v>
+        <f xml:space="preserve"> (X19 - B50) / (P50 - B50)</f>
+        <v>0.21424950458546477</v>
       </c>
       <c r="Q63">
-        <f t="shared" si="17"/>
-        <v>3.0567685589519649E-2</v>
+        <f xml:space="preserve"> (Y19 - B50) / (Q50 - B50)</f>
+        <v>0.19125683060109289</v>
       </c>
     </row>
     <row r="64" spans="2:19" x14ac:dyDescent="0.2">
@@ -3020,60 +2776,60 @@
         <v>4</v>
       </c>
       <c r="D64">
-        <f xml:space="preserve"> (S20 - $B$40) / (C50 - $B$40)</f>
-        <v>0.57358088570993759</v>
+        <f xml:space="preserve"> (S20 - B50) / (C50 - B50)</f>
+        <v>0.57505213270142175</v>
       </c>
       <c r="E64">
-        <f xml:space="preserve"> (U20 - $B$40) / (E50 - $B$40)</f>
-        <v>0.45384615384615384</v>
+        <f xml:space="preserve"> (U20 - B50) / (E50 - B50)</f>
+        <v>0.53518821603927991</v>
       </c>
       <c r="F64">
-        <f t="shared" ref="F64:I64" si="18" xml:space="preserve"> (V20 - $B$40) / (F50 - $B$40)</f>
-        <v>0.51911663773264971</v>
+        <f xml:space="preserve"> (V20 - B50) / (F50 - B50)</f>
+        <v>0.52087691069991959</v>
       </c>
       <c r="G64">
-        <f t="shared" si="18"/>
-        <v>0.43591087003420964</v>
+        <f xml:space="preserve"> (W20 - B50) / (G50 - B50)</f>
+        <v>0.43748847501382998</v>
       </c>
       <c r="H64">
-        <f xml:space="preserve"> (X20 - $B$40) / (H50 - $B$40)</f>
-        <v>0.52358531694132004</v>
+        <f xml:space="preserve"> (X20 - B50) / (H50 - B50)</f>
+        <v>0.52546788831473357</v>
       </c>
       <c r="I64">
-        <f xml:space="preserve"> (Y20 - $B$40) / (I50 - $B$40)</f>
-        <v>0.56078518848985059</v>
+        <f xml:space="preserve"> (Y20 - B50) / (I50 - B50)</f>
+        <v>0.56952339309138611</v>
       </c>
       <c r="J64">
-        <f xml:space="preserve"> (R21 - $B$40) / (J50 - $B$40)</f>
-        <v>0.47476519764681596</v>
+        <f xml:space="preserve"> (R21 - B50) / (J50 - B50)</f>
+        <v>0.47965235173824133</v>
       </c>
       <c r="K64">
-        <f t="shared" ref="K64:Q64" si="19" xml:space="preserve"> (S21 - $B$40) / (K50 - $B$40)</f>
-        <v>0.46328754144954998</v>
+        <f xml:space="preserve"> (S21 - B50) / (K50 - B50)</f>
+        <v>0.4854677565849228</v>
       </c>
       <c r="L64">
-        <f t="shared" si="19"/>
-        <v>0.16121572514040303</v>
+        <f xml:space="preserve"> (T21 - B50) / (L50 - B50)</f>
+        <v>0.18569595894804361</v>
       </c>
       <c r="M64">
-        <f t="shared" si="19"/>
-        <v>0.16844181459566074</v>
+        <f xml:space="preserve"> (U21 - B50) / (M50 - B50)</f>
+        <v>0.17338736030324817</v>
       </c>
       <c r="N64">
-        <f t="shared" si="19"/>
-        <v>0.27196612453084401</v>
+        <f xml:space="preserve"> (V21 - B50) / (N50 - B50)</f>
+        <v>0.27828658652928828</v>
       </c>
       <c r="O64">
-        <f t="shared" si="19"/>
-        <v>0.44497607655502391</v>
+        <f xml:space="preserve"> (W21 - B50) / (O50 - B50)</f>
+        <v>0.44850730615954693</v>
       </c>
       <c r="P64">
-        <f t="shared" si="19"/>
-        <v>0.20844131803035912</v>
+        <f xml:space="preserve"> (X21 - B50) / (P50 - B50)</f>
+        <v>0.21176091064104335</v>
       </c>
       <c r="Q64">
-        <f t="shared" si="19"/>
-        <v>3.4934497816593885E-2</v>
+        <f xml:space="preserve"> (Y21 - B50) / (Q50 - B50)</f>
+        <v>0.19489981785063754</v>
       </c>
     </row>
     <row r="65" spans="2:17" x14ac:dyDescent="0.2">
@@ -3081,124 +2837,124 @@
         <v>5</v>
       </c>
       <c r="D65">
-        <f xml:space="preserve"> (S28 - $B$40) / (C50 - $B$40)</f>
-        <v>0.55417744635519706</v>
+        <f xml:space="preserve"> (S28 - B50) / (C50 - B50)</f>
+        <v>0.55571563981042649</v>
       </c>
       <c r="E65">
-        <f xml:space="preserve"> (U28 - $B$40) / (E50 - $B$40)</f>
-        <v>0.45384615384615384</v>
+        <f xml:space="preserve"> (U28 - B50) / (E50 - B50)</f>
+        <v>0.53518821603927991</v>
       </c>
       <c r="F65">
-        <f t="shared" ref="F65:I65" si="20" xml:space="preserve"> (V28 - $B$40) / (F50 - $B$40)</f>
-        <v>0.50159473535467725</v>
+        <f xml:space="preserve"> (V28 - B50) / (F50 - B50)</f>
+        <v>0.50341914722445691</v>
       </c>
       <c r="G65">
-        <f t="shared" si="20"/>
-        <v>0.42204209942367554</v>
+        <f xml:space="preserve"> (W28 - B50) / (G50 - B50)</f>
+        <v>0.42365849160981006</v>
       </c>
       <c r="H65">
-        <f xml:space="preserve"> (X28 - $B$40) / (H50 - $B$40)</f>
-        <v>0.52803208649402733</v>
+        <f xml:space="preserve"> (X28 - B50) / (H50 - B50)</f>
+        <v>0.52989708628251331</v>
       </c>
       <c r="I65">
-        <f xml:space="preserve"> (Y28 - $B$40) / (I50 - $B$40)</f>
-        <v>0.53714030782957845</v>
+        <f xml:space="preserve"> (Y28 - B50) / (I50 - B50)</f>
+        <v>0.54634892872759078</v>
       </c>
       <c r="J65">
-        <f xml:space="preserve"> (R29 - $B$40) / (J50 - $B$40)</f>
-        <v>0.44318299102074515</v>
+        <f xml:space="preserve"> (R29 - B50) / (J50 - B50)</f>
+        <v>0.44836400817995908</v>
       </c>
       <c r="K65">
-        <f t="shared" ref="K65:P65" si="21" xml:space="preserve"> (S29 - $B$40) / (K50 - $B$40)</f>
-        <v>0.38844149692089058</v>
+        <f xml:space="preserve"> (S29 - B50) / (K50 - B50)</f>
+        <v>0.41371480472297911</v>
       </c>
       <c r="L65">
-        <f t="shared" si="21"/>
-        <v>0.1797158903204493</v>
+        <f xml:space="preserve"> (T29 - B50) / (L50 - B50)</f>
+        <v>0.20365618986529826</v>
       </c>
       <c r="M65">
-        <f t="shared" si="21"/>
-        <v>0.18343195266272189</v>
+        <f xml:space="preserve"> (U29 - B50) / (M50 - B50)</f>
+        <v>0.18828834716685183</v>
       </c>
       <c r="N65">
-        <f t="shared" si="21"/>
-        <v>0.25233375036088923</v>
+        <f xml:space="preserve"> (V29 - B50) / (N50 - B50)</f>
+        <v>0.25882465178401071</v>
       </c>
       <c r="O65">
-        <f t="shared" si="21"/>
-        <v>0.41077962285392627</v>
+        <f xml:space="preserve"> (W29 - B50) / (O50 - B50)</f>
+        <v>0.4145284206110606</v>
       </c>
       <c r="P65">
-        <f t="shared" si="21"/>
-        <v>0.2086264346538319</v>
+        <f xml:space="preserve"> (X29 - B50) / (P50 - B50)</f>
+        <v>0.21194525093322272</v>
       </c>
       <c r="Q65">
-        <f xml:space="preserve"> (Y29 - $B$40) / (Q50 - $B$40)</f>
-        <v>7.8602620087336247E-2</v>
+        <f xml:space="preserve"> (Y29 - B50) / (Q50 - B50)</f>
+        <v>0.23132969034608378</v>
       </c>
     </row>
     <row r="67" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B67" s="13" t="s">
+      <c r="B67" s="12" t="s">
         <v>22</v>
       </c>
       <c r="C67">
         <v>1</v>
       </c>
       <c r="D67">
-        <f xml:space="preserve"> (C18 - $B$43) / (C50 - $B$43)</f>
-        <v>0.39887383959823469</v>
+        <f xml:space="preserve"> (C18 - B50) / (C50 - B50)</f>
+        <v>0.40094786729857818</v>
       </c>
       <c r="E67">
-        <f xml:space="preserve"> (E18 - $B$43) / (E50 - $B$43)</f>
-        <v>0.69230769230769229</v>
+        <f xml:space="preserve"> (E18 - B50) / (E50 - B50)</f>
+        <v>0.73813420621931258</v>
       </c>
       <c r="F67">
-        <f t="shared" ref="F67:H67" si="22" xml:space="preserve"> (F18 - $B$43) / (F50 - $B$43)</f>
-        <v>0.52501110258791228</v>
+        <f xml:space="preserve"> (F18 - B50) / (F50 - B50)</f>
+        <v>0.52674979887369267</v>
       </c>
       <c r="G67">
-        <f t="shared" si="22"/>
-        <v>0.80925817486978768</v>
+        <f xml:space="preserve"> (G18 - B50) / (G50 - B50)</f>
+        <v>0.80979162825004614</v>
       </c>
       <c r="H67">
-        <f t="shared" si="22"/>
-        <v>0.90243264452001049</v>
+        <f xml:space="preserve"> (H18 - B50) / (H50 - B50)</f>
+        <v>0.90281818576577355</v>
       </c>
       <c r="I67">
-        <f xml:space="preserve"> (I18 - $B$43) / (I50 - $B$43)</f>
-        <v>0.86995315636850323</v>
+        <f xml:space="preserve"> (I18 - B50) / (I50 - B50)</f>
+        <v>0.8725404459991255</v>
       </c>
       <c r="J67">
-        <f xml:space="preserve"> (B19 - $B$43) / (J50 - $B$43)</f>
-        <v>0.53091134275983076</v>
+        <f xml:space="preserve"> (B19 - B50) / (J50 - B50)</f>
+        <v>0.53527607361963192</v>
       </c>
       <c r="K67">
-        <f t="shared" ref="K67:P67" si="23" xml:space="preserve"> (C19 - $B$43) / (K50 - $B$43)</f>
-        <v>0.43675982946470865</v>
+        <f xml:space="preserve"> (C19 - B50) / (K50 - B50)</f>
+        <v>0.46003633060853771</v>
       </c>
       <c r="L67">
-        <f t="shared" si="23"/>
-        <v>0.30591344565576478</v>
+        <f xml:space="preserve"> (D19 - B50) / (L50 - B50)</f>
+        <v>0.3261706221937139</v>
       </c>
       <c r="M67">
-        <f t="shared" si="23"/>
-        <v>0.5910585141354372</v>
+        <f xml:space="preserve"> (E19 - B50) / (M50 - B50)</f>
+        <v>0.59349062152800469</v>
       </c>
       <c r="N67">
-        <f t="shared" si="23"/>
-        <v>0.23847560388797998</v>
+        <f xml:space="preserve"> (F19 - B50) / (N50 - B50)</f>
+        <v>0.24508681549322647</v>
       </c>
       <c r="O67">
-        <f t="shared" si="23"/>
-        <v>0.17647058823529413</v>
+        <f xml:space="preserve"> (G19 - B50) / (O50 - B50)</f>
+        <v>0.18171013074180242</v>
       </c>
       <c r="P67">
-        <f t="shared" si="23"/>
-        <v>0.41530914476119957</v>
+        <f xml:space="preserve"> (H19 - B50) / (P50 - B50)</f>
+        <v>0.41776118715148164</v>
       </c>
       <c r="Q67">
-        <f xml:space="preserve"> (I19 - $B$43) / (Q50 - $B$43)</f>
-        <v>0.55895196506550215</v>
+        <f xml:space="preserve"> (I19 - B50) / (Q50 - B50)</f>
+        <v>0.63205828779599271</v>
       </c>
     </row>
     <row r="68" spans="2:17" x14ac:dyDescent="0.2">
@@ -3206,60 +2962,60 @@
         <v>2</v>
       </c>
       <c r="D68">
-        <f xml:space="preserve"> (C20 - $B$43) / (C50 - $B$43)</f>
-        <v>0.52754527469182777</v>
+        <f xml:space="preserve"> (C20 - B50) / (C50 - B50)</f>
+        <v>0.52917535545023697</v>
       </c>
       <c r="E68">
-        <f xml:space="preserve"> (E20 - $B$43) / (E50 - $B$43)</f>
-        <v>0.8</v>
+        <f xml:space="preserve"> (E20 - B50) / (E50 - B50)</f>
+        <v>0.82978723404255317</v>
       </c>
       <c r="F68">
-        <f t="shared" ref="F68:I68" si="24" xml:space="preserve"> (F20 - $B$43) / (F50 - $B$43)</f>
-        <v>0.64217368484799553</v>
+        <f xml:space="preserve"> (F20 - B50) / (F50 - B50)</f>
+        <v>0.64348350764279971</v>
       </c>
       <c r="G68">
-        <f t="shared" si="24"/>
-        <v>0.97784078651339101</v>
+        <f xml:space="preserve"> (G20 - B50) / (G50 - B50)</f>
+        <v>0.97790275985002151</v>
       </c>
       <c r="H68">
-        <f t="shared" si="24"/>
-        <v>0.87583921876362369</v>
+        <f xml:space="preserve"> (H20 - B50) / (H50 - B50)</f>
+        <v>0.87632984497807109</v>
       </c>
       <c r="I68">
-        <f t="shared" si="24"/>
-        <v>0.8891367387909882</v>
+        <f xml:space="preserve"> (I20 - B50) / (I50 - B50)</f>
+        <v>0.89134236991692173</v>
       </c>
       <c r="J68">
-        <f xml:space="preserve"> (B21 - $B$43) / (J50 - $B$43)</f>
-        <v>0.62400660542883679</v>
+        <f xml:space="preserve"> (B21 - B50) / (J50 - B50)</f>
+        <v>0.62750511247443763</v>
       </c>
       <c r="K68">
-        <f t="shared" ref="K68:P68" si="25" xml:space="preserve"> (C21 - $B$43) / (K50 - $B$43)</f>
-        <v>0.58360966366650879</v>
+        <f xml:space="preserve"> (C21 - B50) / (K50 - B50)</f>
+        <v>0.60081743869209814</v>
       </c>
       <c r="L68">
-        <f t="shared" si="25"/>
-        <v>0.3019491245457549</v>
+        <f xml:space="preserve"> (D21 - B50) / (L50 - B50)</f>
+        <v>0.32232200128287364</v>
       </c>
       <c r="M68">
-        <f t="shared" si="25"/>
-        <v>0.59618671926364231</v>
+        <f xml:space="preserve"> (E21 - B50) / (M50 - B50)</f>
+        <v>0.59858832756029012</v>
       </c>
       <c r="N68">
-        <f t="shared" si="25"/>
-        <v>0.34221922817823114</v>
+        <f xml:space="preserve"> (F21 - B50) / (N50 - B50)</f>
+        <v>0.34792978439229155</v>
       </c>
       <c r="O68">
-        <f t="shared" si="25"/>
-        <v>0.30861244019138756</v>
+        <f xml:space="preserve"> (G21 - B50) / (O50 - B50)</f>
+        <v>0.31301125637978044</v>
       </c>
       <c r="P68">
-        <f t="shared" si="25"/>
-        <v>0.4206775268419104</v>
+        <f xml:space="preserve"> (H21 - B50) / (P50 - B50)</f>
+        <v>0.42310705562468315</v>
       </c>
       <c r="Q68">
-        <f xml:space="preserve"> (I21 - $B$43) / (Q50 - $B$43)</f>
-        <v>0.51528384279475981</v>
+        <f xml:space="preserve"> (I21 - B50) / (Q50 - B50)</f>
+        <v>0.59562841530054644</v>
       </c>
     </row>
     <row r="69" spans="2:17" x14ac:dyDescent="0.2">
@@ -3267,60 +3023,60 @@
         <v>3</v>
       </c>
       <c r="D69">
-        <f xml:space="preserve"> (C22 - $B$43) / (C50 - $B$43)</f>
-        <v>0.54200273930908538</v>
+        <f xml:space="preserve"> (C22 - B50) / (C50 - B50)</f>
+        <v>0.54358293838862559</v>
       </c>
       <c r="E69">
-        <f xml:space="preserve"> (E22 - $B$43) / (E50 - $B$43)</f>
-        <v>0.79230769230769227</v>
+        <f xml:space="preserve"> (E22 - B50) / (E50 - B50)</f>
+        <v>0.823240589198036</v>
       </c>
       <c r="F69">
-        <f t="shared" ref="F69:I69" si="26" xml:space="preserve"> (F22 - $B$43) / (F50 - $B$43)</f>
-        <v>0.6237635754370382</v>
+        <f xml:space="preserve"> (F22 - B50) / (F50 - B50)</f>
+        <v>0.62514078841512466</v>
       </c>
       <c r="G69">
-        <f t="shared" si="26"/>
-        <v>0.97747095263044348</v>
+        <f xml:space="preserve"> (G22 - B50) / (G50 - B50)</f>
+        <v>0.97753396029258099</v>
       </c>
       <c r="H69">
-        <f t="shared" si="26"/>
-        <v>0.83799808178568314</v>
+        <f xml:space="preserve"> (H22 - B50) / (H50 - B50)</f>
+        <v>0.83863823874245513</v>
       </c>
       <c r="I69">
-        <f t="shared" si="26"/>
-        <v>0.90073611420923494</v>
+        <f xml:space="preserve"> (I22 - B50) / (I50 - B50)</f>
+        <v>0.90271097507651943</v>
       </c>
       <c r="J69">
-        <f xml:space="preserve"> (B23 - $B$43) / (J50 - $B$43)</f>
-        <v>0.66446485705439162</v>
+        <f xml:space="preserve"> (B23 - B50) / (J50 - B50)</f>
+        <v>0.66758691206543963</v>
       </c>
       <c r="K69">
-        <f t="shared" ref="K69:Q69" si="27" xml:space="preserve"> (C23 - $B$43) / (K50 - $B$43)</f>
-        <v>0.67171956418758882</v>
+        <f xml:space="preserve"> (C23 - B50) / (K50 - B50)</f>
+        <v>0.68528610354223429</v>
       </c>
       <c r="L69">
-        <f t="shared" si="27"/>
-        <v>0.27882391807069706</v>
+        <f xml:space="preserve"> (D23 - B50) / (L50 - B50)</f>
+        <v>0.2998717126363053</v>
       </c>
       <c r="M69">
-        <f t="shared" si="27"/>
-        <v>0.43839579224194608</v>
+        <f xml:space="preserve"> (E23 - B50) / (M50 - B50)</f>
+        <v>0.44173583425919877</v>
       </c>
       <c r="N69">
-        <f t="shared" si="27"/>
-        <v>0.34741603310557212</v>
+        <f xml:space="preserve"> (F23 - B50) / (N50 - B50)</f>
+        <v>0.35308147300133563</v>
       </c>
       <c r="O69">
-        <f t="shared" si="27"/>
-        <v>0.27877849704475094</v>
+        <f xml:space="preserve"> (G23 - B50) / (O50 - B50)</f>
+        <v>0.28336712577780887</v>
       </c>
       <c r="P69">
-        <f t="shared" si="27"/>
-        <v>0.40633098852276933</v>
+        <f xml:space="preserve"> (H23 - B50) / (P50 - B50)</f>
+        <v>0.4088206829807825</v>
       </c>
       <c r="Q69">
-        <f t="shared" si="27"/>
-        <v>0.5633187772925764</v>
+        <f xml:space="preserve"> (I23 - B50) / (Q50 - B50)</f>
+        <v>0.63570127504553731</v>
       </c>
     </row>
     <row r="70" spans="2:17" x14ac:dyDescent="0.2">
@@ -3328,60 +3084,60 @@
         <v>4</v>
       </c>
       <c r="D70">
-        <f xml:space="preserve"> (C26 - $B$43) / (C50 - $B$43)</f>
-        <v>0.60607213513924818</v>
+        <f xml:space="preserve"> (C26 - B50) / (C50 - B50)</f>
+        <v>0.60743127962085308</v>
       </c>
       <c r="E70">
-        <f xml:space="preserve"> (E26 - $B$43) / (E50 - $B$43)</f>
-        <v>0.83461538461538465</v>
+        <f xml:space="preserve"> (E26 - B50) / (E50 - B50)</f>
+        <v>0.85924713584288048</v>
       </c>
       <c r="F70">
-        <f t="shared" ref="F70:I70" si="28" xml:space="preserve"> (F26 - $B$43) / (F50 - $B$43)</f>
-        <v>0.6800436028907102</v>
+        <f xml:space="preserve"> (F26 - B50) / (F50 - B50)</f>
+        <v>0.68121480289621883</v>
       </c>
       <c r="G70">
-        <f t="shared" si="28"/>
-        <v>1.0049619379295467</v>
+        <f xml:space="preserve"> (G26 - B50) / (G50 - B50)</f>
+        <v>1.0049480607289938</v>
       </c>
       <c r="H70">
-        <f t="shared" si="28"/>
-        <v>0.90783852123114483</v>
+        <f xml:space="preserve"> (H26 - B50) / (H50 - B50)</f>
+        <v>0.90820270094229016</v>
       </c>
       <c r="I70">
-        <f t="shared" si="28"/>
-        <v>0.9096587106848093</v>
+        <f xml:space="preserve"> (I26 - B50) / (I50 - B50)</f>
+        <v>0.91145605596851775</v>
       </c>
       <c r="J70">
-        <f xml:space="preserve"> (B27 - $B$43) / (J50 - $B$43)</f>
-        <v>0.68448756321601811</v>
+        <f xml:space="preserve"> (B27 - B50) / (J50 - B50)</f>
+        <v>0.68742331288343561</v>
       </c>
       <c r="K70">
-        <f t="shared" ref="K70:Q70" si="29" xml:space="preserve"> (C27 - $B$43) / (K50 - $B$43)</f>
-        <v>0.6783514921837992</v>
+        <f xml:space="preserve"> (C27 - B50) / (K50 - B50)</f>
+        <v>0.69164396003633066</v>
       </c>
       <c r="L70">
-        <f t="shared" si="29"/>
-        <v>0.33168153287082919</v>
+        <f xml:space="preserve"> (D27 - B50) / (L50 - B50)</f>
+        <v>0.35118665811417576</v>
       </c>
       <c r="M70">
-        <f t="shared" si="29"/>
-        <v>0.68323471400394475</v>
+        <f xml:space="preserve"> (E27 - B50) / (M50 - B50)</f>
+        <v>0.68511861969805898</v>
       </c>
       <c r="N70">
-        <f t="shared" si="29"/>
-        <v>0.3599268597825041</v>
+        <f xml:space="preserve"> (F27 - B50) / (N50 - B50)</f>
+        <v>0.3654836863194047</v>
       </c>
       <c r="O70">
-        <f t="shared" si="29"/>
-        <v>0.28736279200675485</v>
+        <f xml:space="preserve"> (G27 - B50) / (O50 - B50)</f>
+        <v>0.29189680486611203</v>
       </c>
       <c r="P70">
-        <f t="shared" si="29"/>
-        <v>0.46325435024065159</v>
+        <f xml:space="preserve"> (H27 - B50) / (P50 - B50)</f>
+        <v>0.46550532282593665</v>
       </c>
       <c r="Q70">
-        <f t="shared" si="29"/>
-        <v>0.55458515283842791</v>
+        <f xml:space="preserve"> (I27 - B50) / (Q50 - B50)</f>
+        <v>0.62841530054644812</v>
       </c>
     </row>
     <row r="71" spans="2:17" x14ac:dyDescent="0.2">
@@ -3389,124 +3145,124 @@
         <v>5</v>
       </c>
       <c r="D71">
-        <f xml:space="preserve"> (K30 - $B$43) / (C50 - $B$43)</f>
-        <v>0.55105767767463099</v>
+        <f xml:space="preserve"> (K30 - B50) / (C50 - B50)</f>
+        <v>0.55260663507109009</v>
       </c>
       <c r="E71">
-        <f xml:space="preserve"> (M30 - $B$43) / (E50 - $B$43)</f>
-        <v>0.75</v>
+        <f xml:space="preserve"> (M30 - B50) / (E50 - B50)</f>
+        <v>0.78723404255319152</v>
       </c>
       <c r="F71">
-        <f t="shared" ref="F71:I71" si="30" xml:space="preserve"> (N30 - $B$43) / (F50 - $B$43)</f>
-        <v>0.68367717711655696</v>
+        <f xml:space="preserve"> (N30 - B50) / (F50 - B50)</f>
+        <v>0.68483507642799679</v>
       </c>
       <c r="G71">
-        <f t="shared" si="30"/>
-        <v>1.0262273861990323</v>
+        <f xml:space="preserve"> (O30 - B50) / (G50 - B50)</f>
+        <v>1.0261540352818244</v>
       </c>
       <c r="H71">
-        <f t="shared" si="30"/>
-        <v>0.91577295317813234</v>
+        <f xml:space="preserve"> (P30 - B50) / (H50 - B50)</f>
+        <v>0.91610577966911289</v>
       </c>
       <c r="I71">
-        <f t="shared" si="30"/>
-        <v>0.88645995984831583</v>
+        <f xml:space="preserve"> (Q30 - B50) / (I50 - B50)</f>
+        <v>0.88871884564932224</v>
       </c>
       <c r="J71">
-        <f xml:space="preserve"> (J31 - $B$43) / (J50 - $B$43)</f>
-        <v>0.68015275054185154</v>
+        <f xml:space="preserve"> (J31 - B50) / (J50 - B50)</f>
+        <v>0.68312883435582827</v>
       </c>
       <c r="K71">
-        <f t="shared" ref="K71:Q71" si="31" xml:space="preserve"> (K31 - $B$43) / (K50 - $B$43)</f>
-        <v>0.58834675509237333</v>
+        <f xml:space="preserve"> (K31 - B50) / (K50 - B50)</f>
+        <v>0.60535876475930972</v>
       </c>
       <c r="L71">
-        <f t="shared" si="31"/>
-        <v>0.29468120251073671</v>
+        <f xml:space="preserve"> (L31 - B50) / (L50 - B50)</f>
+        <v>0.31526619627966646</v>
       </c>
       <c r="M71">
-        <f t="shared" si="31"/>
-        <v>0.65706771860618018</v>
+        <f xml:space="preserve"> (M31 - B50) / (M50 - B50)</f>
+        <v>0.65910724789229458</v>
       </c>
       <c r="N71">
-        <f t="shared" si="31"/>
-        <v>0.39611202001732271</v>
+        <f xml:space="preserve"> (N31 - B50) / (N50 - B50)</f>
+        <v>0.40135470330089679</v>
       </c>
       <c r="O71">
-        <f t="shared" si="31"/>
-        <v>0.30185758513931887</v>
+        <f xml:space="preserve"> (O31 - B50) / (O50 - B50)</f>
+        <v>0.30629937775291899</v>
       </c>
       <c r="P71">
-        <f t="shared" si="31"/>
-        <v>0.44937060348019253</v>
+        <f xml:space="preserve"> (P31 - B50) / (P50 - B50)</f>
+        <v>0.45167980091248444</v>
       </c>
       <c r="Q71">
-        <f t="shared" si="31"/>
-        <v>0.64192139737991272</v>
+        <f xml:space="preserve"> (Q31 - B50) / (Q50 - B50)</f>
+        <v>0.70127504553734066</v>
       </c>
     </row>
     <row r="73" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B73" s="30" t="s">
+      <c r="B73" s="28" t="s">
         <v>21</v>
       </c>
       <c r="C73">
         <v>1</v>
       </c>
       <c r="D73">
-        <f xml:space="preserve"> (C24 - $B$46) / (C50 - $B$46)</f>
-        <v>0.95022831050228307</v>
+        <f xml:space="preserve"> (C24 - B50) / (C50 - B50)</f>
+        <v>0.95040758293838867</v>
       </c>
       <c r="E73">
-        <f xml:space="preserve"> (E24 - $B$46) / (E50 - $B$46)</f>
-        <v>1.6744186046511629</v>
+        <f xml:space="preserve"> (E24 - B50) / (E50 - B50)</f>
+        <v>1.5695581014729951</v>
       </c>
       <c r="F73">
-        <f t="shared" ref="F73:I73" si="32" xml:space="preserve"> (F24 - $B$46) / (F50 - $B$46)</f>
-        <v>1.3813042600444174</v>
+        <f xml:space="preserve"> (F24 - B50) / (F50 - B50)</f>
+        <v>1.3798471440064359</v>
       </c>
       <c r="G73">
-        <f t="shared" si="32"/>
-        <v>1.0041611441605276</v>
+        <f xml:space="preserve"> (G24 - B50) / (G50 - B50)</f>
+        <v>1.0041489950212059</v>
       </c>
       <c r="H73">
-        <f t="shared" si="32"/>
-        <v>1.1655184442312723</v>
+        <f xml:space="preserve"> (H24 - B50) / (H50 - B50)</f>
+        <v>1.1648356420165877</v>
       </c>
       <c r="I73">
-        <f t="shared" si="32"/>
-        <v>1.3842375530252289</v>
+        <f xml:space="preserve"> (I24 - B50) / (I50 - B50)</f>
+        <v>1.3762571053782247</v>
       </c>
       <c r="J73">
-        <f xml:space="preserve"> (B25 - $B$46) / (J50 - $B$46)</f>
-        <v>1.0740320082601962</v>
+        <f xml:space="preserve"> (B25 - B50) / (J50 - B50)</f>
+        <v>1.0733128834355827</v>
       </c>
       <c r="K73">
-        <f t="shared" ref="K73:P73" si="33" xml:space="preserve"> (C25 - $B$46) / (K50 - $B$46)</f>
-        <v>0.99383009017560509</v>
+        <f xml:space="preserve"> (C25 - B50) / (K50 - B50)</f>
+        <v>0.99409627611262485</v>
       </c>
       <c r="L73">
-        <f t="shared" si="33"/>
-        <v>0.60469732054250747</v>
+        <f xml:space="preserve"> (D25 - B50) / (L50 - B50)</f>
+        <v>0.61674150096215519</v>
       </c>
       <c r="M73">
-        <f t="shared" si="33"/>
-        <v>0.81086413257924506</v>
+        <f xml:space="preserve"> (E25 - B50) / (M50 - B50)</f>
+        <v>0.81203842886085875</v>
       </c>
       <c r="N73">
-        <f t="shared" si="33"/>
-        <v>0.92692789063252146</v>
+        <f xml:space="preserve"> (F25 - B50) / (N50 - B50)</f>
+        <v>0.9275901545506583</v>
       </c>
       <c r="O73">
-        <f t="shared" si="33"/>
-        <v>1.3795045045045045</v>
+        <f xml:space="preserve"> (G25 - B50) / (O50 - B50)</f>
+        <v>1.3769838495420541</v>
       </c>
       <c r="P73">
-        <f t="shared" si="33"/>
-        <v>0.8585447139418626</v>
+        <f xml:space="preserve"> (H25 - B50) / (P50 - B50)</f>
+        <v>0.85916401677496657</v>
       </c>
       <c r="Q73">
-        <f xml:space="preserve"> (I25 - $B$46) / (Q50 - $B$46)</f>
-        <v>1.303964757709251</v>
+        <f xml:space="preserve"> (I25 - B50) / (Q50 - B50)</f>
+        <v>1.2513661202185793</v>
       </c>
     </row>
     <row r="74" spans="2:17" x14ac:dyDescent="0.2">
@@ -3514,60 +3270,60 @@
         <v>2</v>
       </c>
       <c r="D74">
-        <f xml:space="preserve"> (K18 - $B$46) / (C50 - $B$46)</f>
-        <v>0.96971080669710807</v>
+        <f xml:space="preserve"> (K18 - B50) / (C50 - B50)</f>
+        <v>0.96981990521327011</v>
       </c>
       <c r="E74">
-        <f xml:space="preserve"> (M18 - $B$46) / (E50 - $B$46)</f>
-        <v>1.6511627906976745</v>
+        <f xml:space="preserve"> (M18 - B50) / (E50 - B50)</f>
+        <v>1.5499181669394435</v>
       </c>
       <c r="F74">
-        <f t="shared" ref="F74:I74" si="34" xml:space="preserve"> (N18 - $B$46) / (F50 - $B$46)</f>
-        <v>1.3926912982031092</v>
+        <f xml:space="preserve"> (N18 - B50) / (F50 - B50)</f>
+        <v>1.3911906677393404</v>
       </c>
       <c r="G74">
-        <f t="shared" si="34"/>
-        <v>1.0284498967419782</v>
+        <f xml:space="preserve"> (O18 - B50) / (G50 - B50)</f>
+        <v>1.0283668326264674</v>
       </c>
       <c r="H74">
-        <f t="shared" si="34"/>
-        <v>1.163425481817389</v>
+        <f xml:space="preserve"> (P18 - B50) / (H50 - B50)</f>
+        <v>1.162751313561162</v>
       </c>
       <c r="I74">
-        <f t="shared" si="34"/>
-        <v>1.3418173699486493</v>
+        <f xml:space="preserve"> (Q18 - B50) / (I50 - B50)</f>
+        <v>1.3347179711412331</v>
       </c>
       <c r="J74">
-        <f xml:space="preserve"> (J19 - $B$46) / (J50 - $B$46)</f>
-        <v>1.0267423851316468</v>
+        <f xml:space="preserve"> (J19 - B50) / (J50 - B50)</f>
+        <v>1.0264826175869122</v>
       </c>
       <c r="K74">
-        <f t="shared" ref="K74:Q74" si="35" xml:space="preserve"> (K19 - $B$46) / (K50 - $B$46)</f>
-        <v>0.92643569055529185</v>
+        <f xml:space="preserve"> (K19 - B50) / (K50 - B50)</f>
+        <v>0.92960944595821982</v>
       </c>
       <c r="L74">
-        <f t="shared" si="35"/>
-        <v>0.52265960965927882</v>
+        <f xml:space="preserve"> (L19 - B50) / (L50 - B50)</f>
+        <v>0.53720333547145604</v>
       </c>
       <c r="M74">
-        <f t="shared" si="35"/>
-        <v>0.79613310535315007</v>
+        <f xml:space="preserve"> (M19 - B50) / (M50 - B50)</f>
+        <v>0.79739886281942352</v>
       </c>
       <c r="N74">
-        <f t="shared" si="35"/>
-        <v>0.93328198709925869</v>
+        <f xml:space="preserve"> (N19 - B50) / (N50 - B50)</f>
+        <v>0.93388666285060107</v>
       </c>
       <c r="O74">
-        <f t="shared" si="35"/>
-        <v>1.361204954954955</v>
+        <f xml:space="preserve"> (O19 - B50) / (O50 - B50)</f>
+        <v>1.3588058449276375</v>
       </c>
       <c r="P74">
-        <f t="shared" si="35"/>
-        <v>0.84021477504165898</v>
+        <f xml:space="preserve"> (P19 - B50) / (P50 - B50)</f>
+        <v>0.84091432784920961</v>
       </c>
       <c r="Q74">
-        <f t="shared" si="35"/>
-        <v>1.1013215859030836</v>
+        <f xml:space="preserve"> (Q19 - B50) / (Q50 - B50)</f>
+        <v>1.0837887067395264</v>
       </c>
     </row>
     <row r="75" spans="2:17" x14ac:dyDescent="0.2">
@@ -3575,60 +3331,60 @@
         <v>3</v>
       </c>
       <c r="D75">
-        <f xml:space="preserve"> (K26 - $B$46) / (C50 - $B$46)</f>
-        <v>0.98576864535768649</v>
+        <f xml:space="preserve"> (K26 - B50) / (C50 - B50)</f>
+        <v>0.98581990521327012</v>
       </c>
       <c r="E75">
-        <f xml:space="preserve"> (M26 - $B$46) / (E50 - $B$46)</f>
-        <v>1.6705426356589148</v>
+        <f xml:space="preserve"> (M26 - B50) / (E50 - B50)</f>
+        <v>1.5662847790507366</v>
       </c>
       <c r="F75">
-        <f t="shared" ref="F75:I75" si="36" xml:space="preserve"> (N26 - $B$46) / (F50 - $B$46)</f>
-        <v>1.4356551584898041</v>
+        <f xml:space="preserve"> (N26 - B50) / (F50 - B50)</f>
+        <v>1.4339903459372485</v>
       </c>
       <c r="G75">
-        <f t="shared" si="36"/>
-        <v>0.9911537157476189</v>
+        <f xml:space="preserve"> (O26 - B50) / (G50 - B50)</f>
+        <v>0.99117954391788066</v>
       </c>
       <c r="H75">
-        <f t="shared" si="36"/>
-        <v>1.1689195081538328</v>
+        <f xml:space="preserve"> (P26 - B50) / (H50 - B50)</f>
+        <v>1.1682226757566547</v>
       </c>
       <c r="I75">
-        <f t="shared" si="36"/>
-        <v>1.3757535164099128</v>
+        <f xml:space="preserve"> (Q26 - B50) / (I50 - B50)</f>
+        <v>1.3679492785308265</v>
       </c>
       <c r="J75">
-        <f xml:space="preserve"> (J27 - $B$46) / (J50 - $B$46)</f>
-        <v>1.1397005678884873</v>
+        <f xml:space="preserve"> (J27 - B50) / (J50 - B50)</f>
+        <v>1.1383435582822086</v>
       </c>
       <c r="K75">
-        <f t="shared" ref="K75:Q75" si="37" xml:space="preserve"> (K27 - $B$46) / (K50 - $B$46)</f>
-        <v>0.8998576174655909</v>
+        <f xml:space="preserve"> (K27 - B50) / (K50 - B50)</f>
+        <v>0.90417801998183467</v>
       </c>
       <c r="L75">
-        <f t="shared" si="37"/>
-        <v>0.53986106516705257</v>
+        <f xml:space="preserve"> (L27 - B50) / (L50 - B50)</f>
+        <v>0.55388069275176399</v>
       </c>
       <c r="M75">
-        <f t="shared" si="37"/>
-        <v>0.82848875443903724</v>
+        <f xml:space="preserve"> (M27 - B50) / (M50 - B50)</f>
+        <v>0.82955362394614729</v>
       </c>
       <c r="N75">
-        <f t="shared" si="37"/>
-        <v>0.93097140656589972</v>
+        <f xml:space="preserve"> (N27 - B50) / (N50 - B50)</f>
+        <v>0.93159702346880369</v>
       </c>
       <c r="O75">
-        <f t="shared" si="37"/>
-        <v>1.3918918918918919</v>
+        <f xml:space="preserve"> (O27 - B50) / (O50 - B50)</f>
+        <v>1.3892889603579668</v>
       </c>
       <c r="P75">
-        <f t="shared" si="37"/>
-        <v>0.85947046843177188</v>
+        <f xml:space="preserve"> (P27 - B50) / (P50 - B50)</f>
+        <v>0.86008571823586344</v>
       </c>
       <c r="Q75">
-        <f t="shared" si="37"/>
-        <v>1.2819383259911894</v>
+        <f xml:space="preserve"> (Q27 - B50) / (Q50 - B50)</f>
+        <v>1.2331511839708562</v>
       </c>
     </row>
     <row r="76" spans="2:17" x14ac:dyDescent="0.2">
@@ -3636,60 +3392,60 @@
         <v>4</v>
       </c>
       <c r="D76">
-        <f xml:space="preserve"> (S16 - $B$46) / (C50 - $B$46)</f>
-        <v>0.75</v>
+        <f xml:space="preserve"> (S16 - B50) / (C50 - B50)</f>
+        <v>0.75090047393364934</v>
       </c>
       <c r="E76">
-        <f xml:space="preserve"> (U16 - $B$46) / (E50 - $B$46)</f>
-        <v>1.3527131782945736</v>
+        <f xml:space="preserve"> (U16 - B50) / (E50 - B50)</f>
+        <v>1.2978723404255319</v>
       </c>
       <c r="F76">
-        <f t="shared" ref="F76:I76" si="38" xml:space="preserve"> (V16 - $B$46) / (F50 - $B$46)</f>
-        <v>1.1310316979608319</v>
+        <f xml:space="preserve"> (V16 - B50) / (F50 - B50)</f>
+        <v>1.1305309734513274</v>
       </c>
       <c r="G76">
-        <f t="shared" si="38"/>
-        <v>0.81126899485251058</v>
+        <f xml:space="preserve"> (W16 - B50) / (G50 - B50)</f>
+        <v>0.81182002581596902</v>
       </c>
       <c r="H76">
-        <f t="shared" si="38"/>
-        <v>1.1535711171186884</v>
+        <f xml:space="preserve"> (X16 - B50) / (H50 - B50)</f>
+        <v>1.1529376004168657</v>
       </c>
       <c r="I76">
-        <f t="shared" si="38"/>
-        <v>1.400312569770038</v>
+        <f xml:space="preserve"> (Y16 - B50) / (I50 - B50)</f>
+        <v>1.3919982509838216</v>
       </c>
       <c r="J76">
-        <f xml:space="preserve"> (R17 - $B$46) / (J50 - $B$46)</f>
-        <v>0.89478575116159009</v>
+        <f xml:space="preserve"> (R17 - B50) / (J50 - B50)</f>
+        <v>0.89580777096114517</v>
       </c>
       <c r="K76">
-        <f t="shared" ref="K76:Q76" si="39" xml:space="preserve"> (S17 - $B$46) / (K50 - $B$46)</f>
-        <v>0.66635026103464645</v>
+        <f xml:space="preserve"> (S17 - B50) / (K50 - B50)</f>
+        <v>0.68074477747502271</v>
       </c>
       <c r="L76">
-        <f t="shared" si="39"/>
-        <v>0.41746609328481643</v>
+        <f xml:space="preserve"> (T17 - B50) / (L50 - B50)</f>
+        <v>0.43521488133418856</v>
       </c>
       <c r="M76">
-        <f t="shared" si="39"/>
-        <v>0.65342627910035511</v>
+        <f xml:space="preserve"> (U17 - B50) / (M50 - B50)</f>
+        <v>0.65557806679302011</v>
       </c>
       <c r="N76">
-        <f xml:space="preserve"> (V17 - $B$46) / (N50 - $B$46)</f>
-        <v>0.68316164436314619</v>
+        <f xml:space="preserve"> (V17 - B50) / (N50 - B50)</f>
+        <v>0.68603319977103605</v>
       </c>
       <c r="O76">
-        <f t="shared" si="39"/>
-        <v>0.9911317567567568</v>
+        <f xml:space="preserve"> (W17 - B50) / (O50 - B50)</f>
+        <v>0.99119065930224426</v>
       </c>
       <c r="P76">
-        <f t="shared" si="39"/>
-        <v>0.84141825587854102</v>
+        <f xml:space="preserve"> (X17 - B50) / (P50 - B50)</f>
+        <v>0.84211253974837552</v>
       </c>
       <c r="Q76">
-        <f t="shared" si="39"/>
-        <v>0.99559471365638763</v>
+        <f xml:space="preserve"> (Y17 - B50) / (Q50 - B50)</f>
+        <v>0.99635701275045541</v>
       </c>
     </row>
     <row r="77" spans="2:17" x14ac:dyDescent="0.2">
@@ -3697,60 +3453,60 @@
         <v>5</v>
       </c>
       <c r="D77">
-        <f xml:space="preserve"> (K22 - $B$46) / (C50 - $B$46)</f>
-        <v>1.0030441400304415</v>
+        <f xml:space="preserve"> (K22 - B50) / (C50 - B50)</f>
+        <v>1.0030331753554502</v>
       </c>
       <c r="E77">
-        <f xml:space="preserve"> (M22 - $B$46) / (E50 - $B$46)</f>
-        <v>1.682170542635659</v>
+        <f xml:space="preserve"> (M22 - B50) / (E50 - B50)</f>
+        <v>1.5761047463175122</v>
       </c>
       <c r="F77">
-        <f t="shared" ref="F77:I77" si="40" xml:space="preserve"> (N22 - $B$46) / (F50 - $B$46)</f>
-        <v>1.3817080557238037</v>
+        <f xml:space="preserve"> (N22 - B50) / (F50 - B50)</f>
+        <v>1.380249396621078</v>
       </c>
       <c r="G77">
-        <f t="shared" si="40"/>
-        <v>1.023579816909657</v>
+        <f xml:space="preserve"> (O22 - B50) / (G50 - B50)</f>
+        <v>1.0235109717868338</v>
       </c>
       <c r="H77">
-        <f xml:space="preserve"> (P22 - $B$46) / (H50 - $B$46)</f>
-        <v>1.1751983953954828</v>
+        <f xml:space="preserve"> (P22 - B50) / (H50 - B50)</f>
+        <v>1.1744756611229319</v>
       </c>
       <c r="I77">
-        <f t="shared" si="40"/>
-        <v>1.3324402768475105</v>
+        <f xml:space="preserve"> (Q22 - B50) / (I50 - B50)</f>
+        <v>1.3255356362046349</v>
       </c>
       <c r="J77">
-        <f xml:space="preserve"> (J23 - $B$46) / (J50 - $B$46)</f>
-        <v>1.0996386164171399</v>
+        <f xml:space="preserve"> (J23 - B50) / (J50 - B50)</f>
+        <v>1.0986707566462168</v>
       </c>
       <c r="K77">
-        <f t="shared" ref="K77:Q77" si="41" xml:space="preserve"> (K23 - $B$46) / (K50 - $B$46)</f>
-        <v>0.97959183673469385</v>
+        <f xml:space="preserve"> (K23 - B50) / (K50 - B50)</f>
+        <v>0.98047229791099</v>
       </c>
       <c r="L77">
-        <f t="shared" si="41"/>
-        <v>0.51405888190539195</v>
+        <f xml:space="preserve"> (L23 - B50) / (L50 - B50)</f>
+        <v>0.52886465683130213</v>
       </c>
       <c r="M77">
-        <f t="shared" si="41"/>
-        <v>0.8062606865710904</v>
+        <f xml:space="preserve"> (M23 - B50) / (M50 - B50)</f>
+        <v>0.80746356447291023</v>
       </c>
       <c r="N77">
-        <f t="shared" si="41"/>
-        <v>0.88957350534321744</v>
+        <f xml:space="preserve"> (N23 - B50) / (N50 - B50)</f>
+        <v>0.89057431787826746</v>
       </c>
       <c r="O77">
-        <f t="shared" si="41"/>
-        <v>1.3460022522522523</v>
+        <f xml:space="preserve"> (O23 - B50) / (O50 - B50)</f>
+        <v>1.3437041180171991</v>
       </c>
       <c r="P77">
-        <f t="shared" si="41"/>
-        <v>0.79503795593408633</v>
+        <f xml:space="preserve"> (P23 - B50) / (P50 - B50)</f>
+        <v>0.79593529655744499</v>
       </c>
       <c r="Q77">
-        <f t="shared" si="41"/>
-        <v>1.0704845814977975</v>
+        <f xml:space="preserve"> (Q23 - B50) / (Q50 - B50)</f>
+        <v>1.0582877959927139</v>
       </c>
     </row>
   </sheetData>
@@ -3797,13 +3553,13 @@
       <c r="A4" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C4" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="17" t="s">
         <v>21</v>
       </c>
     </row>
@@ -3811,13 +3567,13 @@
       <c r="A5" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="22" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3825,13 +3581,13 @@
       <c r="A6" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="22" t="s">
         <v>20</v>
       </c>
       <c r="K6" s="3"/>
@@ -3841,10 +3597,10 @@
       <c r="A7" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="17" t="s">
         <v>21</v>
       </c>
       <c r="D7" t="s">
@@ -3857,13 +3613,13 @@
       <c r="A8" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="17" t="s">
         <v>21</v>
       </c>
       <c r="C8" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>18</v>
       </c>
       <c r="K8" s="3"/>
@@ -3873,10 +3629,10 @@
       <c r="A9" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="17" t="s">
         <v>21</v>
       </c>
       <c r="D9" t="s">
@@ -3889,13 +3645,13 @@
       <c r="A10" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="23" t="s">
+      <c r="D10" s="22" t="s">
         <v>20</v>
       </c>
       <c r="K10" s="3"/>
@@ -3905,13 +3661,13 @@
       <c r="A11" t="s">
         <v>58</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="7" t="s">
         <v>18</v>
       </c>
       <c r="K11" s="3"/>

</xml_diff>